<commit_message>
Update Leave Card 1/4/2024 4:38 PM
</commit_message>
<xml_diff>
--- a/CASUAL/LA ACCOUNTING/ABELA, IMELDA.xlsx
+++ b/CASUAL/LA ACCOUNTING/ABELA, IMELDA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA ACCOUNTING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA ACCOUNTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC45DE8-C87F-4829-BF4E-31978707C9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018 LEAVE CREDITS" sheetId="4" r:id="rId1"/>
@@ -26,7 +27,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="161">
   <si>
     <t>PERIOD</t>
   </si>
@@ -524,7 +525,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -902,14 +903,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -919,9 +923,6 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1433,7 +1434,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1450,25 +1451,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K120" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K120" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="23"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="22"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="20"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1480,25 +1481,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K204" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K204" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1805,34 +1806,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A82" activePane="bottomLeft"/>
+      <pane ySplit="3696" topLeftCell="A85" activePane="bottomLeft"/>
       <selection activeCell="I9" sqref="I9"/>
-      <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
+      <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -1844,16 +1845,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -1862,18 +1863,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="55">
         <v>43101</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -1884,16 +1885,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -1901,7 +1902,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -1914,24 +1915,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -1966,7 +1967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -1985,12 +1986,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
-        <v>88.75</v>
+        <v>87.75</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>43</v>
       </c>
@@ -2012,7 +2013,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="41">
         <v>43101</v>
       </c>
@@ -2032,7 +2033,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="41">
         <v>43132</v>
       </c>
@@ -2058,7 +2059,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="41">
         <v>43160</v>
       </c>
@@ -2078,7 +2079,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="41">
         <v>43191</v>
       </c>
@@ -2098,7 +2099,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="41">
         <v>43221</v>
       </c>
@@ -2118,7 +2119,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="41">
         <v>43252</v>
       </c>
@@ -2138,7 +2139,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="41">
         <v>43282</v>
       </c>
@@ -2158,7 +2159,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="41">
         <v>43313</v>
       </c>
@@ -2178,7 +2179,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="41">
         <v>43344</v>
       </c>
@@ -2198,7 +2199,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="41">
         <v>43374</v>
       </c>
@@ -2218,7 +2219,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="41">
         <v>43405</v>
       </c>
@@ -2238,7 +2239,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="41">
         <v>43435</v>
       </c>
@@ -2258,7 +2259,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="47" t="s">
         <v>44</v>
       </c>
@@ -2276,7 +2277,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="41">
         <v>43466</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="41">
         <v>43497</v>
       </c>
@@ -2322,7 +2323,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="41">
         <v>43525</v>
       </c>
@@ -2342,7 +2343,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="41">
         <v>43556</v>
       </c>
@@ -2362,7 +2363,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="41">
         <v>43586</v>
       </c>
@@ -2382,7 +2383,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="41">
         <v>43617</v>
       </c>
@@ -2402,7 +2403,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="41">
         <v>43647</v>
       </c>
@@ -2422,7 +2423,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="41">
         <v>43678</v>
       </c>
@@ -2442,7 +2443,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="41">
         <v>43709</v>
       </c>
@@ -2462,7 +2463,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="41">
         <v>43739</v>
       </c>
@@ -2482,7 +2483,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="41">
         <v>43770</v>
       </c>
@@ -2502,7 +2503,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="41">
         <v>43800</v>
       </c>
@@ -2522,7 +2523,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="47" t="s">
         <v>45</v>
       </c>
@@ -2540,7 +2541,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="41">
         <v>43831</v>
       </c>
@@ -2564,7 +2565,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="41">
         <v>43862</v>
       </c>
@@ -2584,7 +2585,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="41">
         <v>43891</v>
       </c>
@@ -2604,7 +2605,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="41">
         <v>43922</v>
       </c>
@@ -2624,7 +2625,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="41">
         <v>43952</v>
       </c>
@@ -2644,7 +2645,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="41">
         <v>43983</v>
       </c>
@@ -2664,7 +2665,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="41">
         <v>44013</v>
       </c>
@@ -2684,7 +2685,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="41">
         <v>44044</v>
       </c>
@@ -2704,7 +2705,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="41">
         <v>44075</v>
       </c>
@@ -2724,7 +2725,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="41">
         <v>44105</v>
       </c>
@@ -2744,7 +2745,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="41">
         <v>44136</v>
       </c>
@@ -2764,7 +2765,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="41">
         <v>44166</v>
       </c>
@@ -2784,7 +2785,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="47" t="s">
         <v>46</v>
       </c>
@@ -2802,7 +2803,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="41">
         <v>44197</v>
       </c>
@@ -2822,7 +2823,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="41">
         <v>44228</v>
       </c>
@@ -2846,7 +2847,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="41"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13">
@@ -2864,7 +2865,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="41">
         <v>44256</v>
       </c>
@@ -2884,7 +2885,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="41">
         <v>44287</v>
       </c>
@@ -2904,7 +2905,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="41">
         <v>44317</v>
       </c>
@@ -2924,7 +2925,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="41">
         <v>44348</v>
       </c>
@@ -2944,7 +2945,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="41">
         <v>44378</v>
       </c>
@@ -2964,7 +2965,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="41">
         <v>44409</v>
       </c>
@@ -2984,7 +2985,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="41">
         <v>44440</v>
       </c>
@@ -3004,7 +3005,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="41">
         <v>44470</v>
       </c>
@@ -3030,7 +3031,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="41">
         <v>44501</v>
       </c>
@@ -3050,7 +3051,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="41">
         <v>44531</v>
       </c>
@@ -3070,7 +3071,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="47" t="s">
         <v>52</v>
       </c>
@@ -3088,7 +3089,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="41">
         <v>44562</v>
       </c>
@@ -3108,7 +3109,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="41">
         <v>44593</v>
       </c>
@@ -3128,7 +3129,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="41">
         <v>44621</v>
       </c>
@@ -3152,7 +3153,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="41">
         <v>44652</v>
       </c>
@@ -3172,7 +3173,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="41"/>
       <c r="B68" s="20" t="s">
         <v>155</v>
@@ -3192,7 +3193,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="41">
         <v>44682</v>
       </c>
@@ -3216,7 +3217,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="41">
         <v>44713</v>
       </c>
@@ -3240,7 +3241,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="41">
         <v>44743</v>
       </c>
@@ -3264,7 +3265,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="41">
         <v>44774</v>
       </c>
@@ -3288,7 +3289,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="41">
         <v>44805</v>
       </c>
@@ -3312,7 +3313,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="41">
         <v>44835</v>
       </c>
@@ -3338,7 +3339,7 @@
         <v>44855</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="41"/>
       <c r="B75" s="20" t="s">
         <v>149</v>
@@ -3358,7 +3359,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="48"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="41">
         <v>44866</v>
       </c>
@@ -3384,7 +3385,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="41"/>
       <c r="B77" s="20" t="s">
         <v>62</v>
@@ -3406,7 +3407,7 @@
         <v>44894</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="41">
         <v>44896</v>
       </c>
@@ -3430,7 +3431,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="47" t="s">
         <v>145</v>
       </c>
@@ -3448,7 +3449,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="41">
         <v>44927</v>
       </c>
@@ -3474,7 +3475,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="41">
         <v>44958</v>
       </c>
@@ -3494,7 +3495,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="41">
         <v>44986</v>
       </c>
@@ -3514,7 +3515,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="41">
         <v>45017</v>
       </c>
@@ -3534,7 +3535,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="41">
         <v>45047</v>
       </c>
@@ -3554,7 +3555,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="41">
         <v>45078</v>
       </c>
@@ -3574,7 +3575,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="41">
         <v>45108</v>
       </c>
@@ -3594,7 +3595,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="41">
         <v>45139</v>
       </c>
@@ -3614,7 +3615,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="48"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="41">
         <v>45170</v>
       </c>
@@ -3634,7 +3635,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="41">
         <v>45200</v>
       </c>
@@ -3660,7 +3661,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="41">
         <v>45231</v>
       </c>
@@ -3684,7 +3685,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="41">
         <v>45261</v>
       </c>
@@ -3706,7 +3707,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="41"/>
       <c r="B92" s="20" t="s">
         <v>158</v>
@@ -3728,7 +3729,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="47" t="s">
         <v>157</v>
       </c>
@@ -3746,11 +3747,13 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="41">
         <v>45292</v>
       </c>
-      <c r="B94" s="20"/>
+      <c r="B94" s="20" t="s">
+        <v>57</v>
+      </c>
       <c r="C94" s="13"/>
       <c r="D94" s="40"/>
       <c r="E94" s="9"/>
@@ -3759,12 +3762,16 @@
         <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H94" s="40"/>
+      <c r="H94" s="40">
+        <v>1</v>
+      </c>
       <c r="I94" s="9"/>
       <c r="J94" s="11"/>
-      <c r="K94" s="20"/>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K94" s="48">
+        <v>45293</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="41">
         <v>45323</v>
       </c>
@@ -3782,7 +3789,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="41">
         <v>45352</v>
       </c>
@@ -3800,7 +3807,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="41">
         <v>45383</v>
       </c>
@@ -3818,7 +3825,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="41">
         <v>45413</v>
       </c>
@@ -3836,7 +3843,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="41">
         <v>45444</v>
       </c>
@@ -3854,7 +3861,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="41">
         <v>45474</v>
       </c>
@@ -3872,7 +3879,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="41"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -3888,7 +3895,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="41"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -3904,7 +3911,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="41"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -3920,7 +3927,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="41"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -3936,7 +3943,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="41"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -3952,7 +3959,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="41"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -3968,7 +3975,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="41"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -3984,7 +3991,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="41"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4000,7 +4007,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="41"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -4016,7 +4023,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="41"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -4032,7 +4039,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="41"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -4048,7 +4055,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="41"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -4064,7 +4071,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="41"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -4080,7 +4087,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="41"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -4096,7 +4103,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="41"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -4112,7 +4119,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="41"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -4128,7 +4135,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="41"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -4144,7 +4151,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="41"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -4160,7 +4167,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="41"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -4176,7 +4183,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="42"/>
       <c r="B120" s="15"/>
       <c r="C120" s="43"/>
@@ -4194,23 +4201,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4233,34 +4240,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K204"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3990" topLeftCell="A162" activePane="bottomLeft"/>
+      <pane ySplit="3984" topLeftCell="A162" activePane="bottomLeft"/>
       <selection activeCell="I9" sqref="I9"/>
       <selection pane="bottomLeft" activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -4272,16 +4279,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -4290,18 +4297,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="55">
         <v>43101</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -4312,16 +4319,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -4329,7 +4336,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -4342,24 +4349,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -4394,7 +4401,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -4418,7 +4425,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>43</v>
       </c>
@@ -4440,7 +4447,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="41">
         <v>43101</v>
       </c>
@@ -4462,7 +4469,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="41"/>
       <c r="B12" s="20" t="s">
         <v>57</v>
@@ -4484,7 +4491,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="41"/>
       <c r="B13" s="20" t="s">
         <v>66</v>
@@ -4504,7 +4511,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
       <c r="B14" s="20" t="s">
         <v>55</v>
@@ -4526,7 +4533,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="41">
         <v>43132</v>
       </c>
@@ -4548,7 +4555,7 @@
         <v>43138</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="20" t="s">
         <v>57</v>
@@ -4570,7 +4577,7 @@
         <v>43133</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="41"/>
       <c r="B17" s="20" t="s">
         <v>57</v>
@@ -4592,7 +4599,7 @@
         <v>43117</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="41"/>
       <c r="B18" s="20" t="s">
         <v>57</v>
@@ -4612,7 +4619,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="48"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="41"/>
       <c r="B19" s="20" t="s">
         <v>57</v>
@@ -4634,7 +4641,7 @@
         <v>43146</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="41"/>
       <c r="B20" s="20" t="s">
         <v>55</v>
@@ -4656,7 +4663,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="41"/>
       <c r="B21" s="20" t="s">
         <v>57</v>
@@ -4678,7 +4685,7 @@
         <v>43159</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="41">
         <v>43160</v>
       </c>
@@ -4700,7 +4707,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="41"/>
       <c r="B23" s="20" t="s">
         <v>71</v>
@@ -4722,7 +4729,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="41"/>
       <c r="B24" s="20" t="s">
         <v>55</v>
@@ -4744,7 +4751,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="41">
         <v>43191</v>
       </c>
@@ -4768,7 +4775,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="41"/>
       <c r="B26" s="20" t="s">
         <v>57</v>
@@ -4790,7 +4797,7 @@
         <v>43203</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="41"/>
       <c r="B27" s="20" t="s">
         <v>55</v>
@@ -4812,7 +4819,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="41"/>
       <c r="B28" s="20" t="s">
         <v>71</v>
@@ -4834,7 +4841,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="41"/>
       <c r="B29" s="20" t="s">
         <v>75</v>
@@ -4856,7 +4863,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="41"/>
       <c r="B30" s="20" t="s">
         <v>55</v>
@@ -4878,7 +4885,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="41">
         <v>43221</v>
       </c>
@@ -4902,7 +4909,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="41"/>
       <c r="B32" s="15" t="s">
         <v>71</v>
@@ -4924,7 +4931,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="41"/>
       <c r="B33" s="15" t="s">
         <v>71</v>
@@ -4946,7 +4953,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="41"/>
       <c r="B34" s="15" t="s">
         <v>84</v>
@@ -4966,7 +4973,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="15"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="41">
         <v>43252</v>
       </c>
@@ -4990,7 +4997,7 @@
         <v>43258</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="41"/>
       <c r="B36" s="15" t="s">
         <v>57</v>
@@ -5012,7 +5019,7 @@
         <v>43270</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="41"/>
       <c r="B37" s="15" t="s">
         <v>57</v>
@@ -5034,7 +5041,7 @@
         <v>43276</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="41"/>
       <c r="B38" s="15" t="s">
         <v>85</v>
@@ -5054,7 +5061,7 @@
       <c r="J38" s="12"/>
       <c r="K38" s="49"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="41">
         <v>43282</v>
       </c>
@@ -5078,7 +5085,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="41"/>
       <c r="B40" s="20" t="s">
         <v>57</v>
@@ -5098,7 +5105,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="41"/>
       <c r="B41" s="20" t="s">
         <v>87</v>
@@ -5118,7 +5125,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="41">
         <v>43313</v>
       </c>
@@ -5142,7 +5149,7 @@
         <v>43318</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="41"/>
       <c r="B43" s="20" t="s">
         <v>57</v>
@@ -5164,7 +5171,7 @@
         <v>43325</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="41"/>
       <c r="B44" s="20" t="s">
         <v>57</v>
@@ -5186,7 +5193,7 @@
         <v>43328</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="41"/>
       <c r="B45" s="20" t="s">
         <v>88</v>
@@ -5206,7 +5213,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="48"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="41">
         <v>43344</v>
       </c>
@@ -5230,7 +5237,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="41"/>
       <c r="B47" s="20" t="s">
         <v>55</v>
@@ -5252,7 +5259,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="41"/>
       <c r="B48" s="20" t="s">
         <v>90</v>
@@ -5270,7 +5277,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="48"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="41">
         <v>43374</v>
       </c>
@@ -5294,7 +5301,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="41"/>
       <c r="B50" s="20" t="s">
         <v>75</v>
@@ -5316,7 +5323,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="41"/>
       <c r="B51" s="20" t="s">
         <v>93</v>
@@ -5336,7 +5343,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="41">
         <v>43405</v>
       </c>
@@ -5360,7 +5367,7 @@
         <v>43425</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="41"/>
       <c r="B53" s="20" t="s">
         <v>55</v>
@@ -5382,7 +5389,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="41"/>
       <c r="B54" s="20" t="s">
         <v>95</v>
@@ -5400,7 +5407,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="48"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="41">
         <v>43435</v>
       </c>
@@ -5424,7 +5431,7 @@
         <v>43452</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="41"/>
       <c r="B56" s="20" t="s">
         <v>57</v>
@@ -5446,7 +5453,7 @@
         <v>43445</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="41"/>
       <c r="B57" s="20" t="s">
         <v>55</v>
@@ -5468,7 +5475,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="41"/>
       <c r="B58" s="20" t="s">
         <v>97</v>
@@ -5486,7 +5493,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="48"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="47" t="s">
         <v>44</v>
       </c>
@@ -5504,7 +5511,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="41">
         <v>43466</v>
       </c>
@@ -5526,7 +5533,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="41"/>
       <c r="B61" s="20" t="s">
         <v>71</v>
@@ -5548,7 +5555,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="41">
         <v>43497</v>
       </c>
@@ -5572,7 +5579,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="41"/>
       <c r="B63" s="20" t="s">
         <v>57</v>
@@ -5594,7 +5601,7 @@
         <v>43517</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="41"/>
       <c r="B64" s="20" t="s">
         <v>53</v>
@@ -5614,7 +5621,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="41"/>
       <c r="B65" s="20" t="s">
         <v>55</v>
@@ -5636,7 +5643,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="41">
         <v>43525</v>
       </c>
@@ -5660,7 +5667,7 @@
         <v>43531</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="41"/>
       <c r="B67" s="20" t="s">
         <v>71</v>
@@ -5682,7 +5689,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="41"/>
       <c r="B68" s="20" t="s">
         <v>57</v>
@@ -5704,7 +5711,7 @@
         <v>43552</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="41">
         <v>43556</v>
       </c>
@@ -5728,7 +5735,7 @@
         <v>43817</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="41"/>
       <c r="B70" s="20" t="s">
         <v>57</v>
@@ -5750,7 +5757,7 @@
         <v>43557</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="41"/>
       <c r="B71" s="20" t="s">
         <v>57</v>
@@ -5772,7 +5779,7 @@
         <v>43572</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="41"/>
       <c r="B72" s="20" t="s">
         <v>55</v>
@@ -5794,7 +5801,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="41">
         <v>43586</v>
       </c>
@@ -5818,7 +5825,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="41"/>
       <c r="B74" s="20" t="s">
         <v>75</v>
@@ -5840,7 +5847,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="41"/>
       <c r="B75" s="20" t="s">
         <v>57</v>
@@ -5862,7 +5869,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="41"/>
       <c r="B76" s="20" t="s">
         <v>57</v>
@@ -5884,7 +5891,7 @@
         <v>43601</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="41"/>
       <c r="B77" s="20" t="s">
         <v>55</v>
@@ -5906,7 +5913,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="41"/>
       <c r="B78" s="20" t="s">
         <v>57</v>
@@ -5928,7 +5935,7 @@
         <v>43615</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="41">
         <v>43617</v>
       </c>
@@ -5952,7 +5959,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="41"/>
       <c r="B80" s="20" t="s">
         <v>71</v>
@@ -5974,7 +5981,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="41"/>
       <c r="B81" s="20" t="s">
         <v>57</v>
@@ -5996,7 +6003,7 @@
         <v>43629</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="41"/>
       <c r="B82" s="20" t="s">
         <v>57</v>
@@ -6018,7 +6025,7 @@
         <v>43633</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="41"/>
       <c r="B83" s="20" t="s">
         <v>108</v>
@@ -6040,7 +6047,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="41"/>
       <c r="B84" s="20" t="s">
         <v>66</v>
@@ -6060,7 +6067,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="41">
         <v>43647</v>
       </c>
@@ -6084,7 +6091,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="41"/>
       <c r="B86" s="20" t="s">
         <v>57</v>
@@ -6106,7 +6113,7 @@
         <v>43663</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="41"/>
       <c r="B87" s="20" t="s">
         <v>57</v>
@@ -6128,7 +6135,7 @@
         <v>43668</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="41">
         <v>43678</v>
       </c>
@@ -6152,7 +6159,7 @@
         <v>43678</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="41"/>
       <c r="B89" s="20" t="s">
         <v>57</v>
@@ -6174,7 +6181,7 @@
         <v>43685</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="41"/>
       <c r="B90" s="20" t="s">
         <v>57</v>
@@ -6196,7 +6203,7 @@
         <v>43700</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="41"/>
       <c r="B91" s="20" t="s">
         <v>55</v>
@@ -6218,7 +6225,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="41">
         <v>43709</v>
       </c>
@@ -6242,7 +6249,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="41"/>
       <c r="B93" s="20" t="s">
         <v>55</v>
@@ -6264,7 +6271,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="41"/>
       <c r="B94" s="20" t="s">
         <v>55</v>
@@ -6286,7 +6293,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="41">
         <v>43739</v>
       </c>
@@ -6310,7 +6317,7 @@
         <v>43749</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="41"/>
       <c r="B96" s="20" t="s">
         <v>55</v>
@@ -6332,7 +6339,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="41"/>
       <c r="B97" s="20" t="s">
         <v>57</v>
@@ -6354,7 +6361,7 @@
         <v>43755</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="41"/>
       <c r="B98" s="20" t="s">
         <v>57</v>
@@ -6376,7 +6383,7 @@
         <v>43762</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="41"/>
       <c r="B99" s="20" t="s">
         <v>57</v>
@@ -6398,7 +6405,7 @@
         <v>43769</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="41">
         <v>43770</v>
       </c>
@@ -6422,7 +6429,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="41"/>
       <c r="B101" s="20" t="s">
         <v>57</v>
@@ -6444,7 +6451,7 @@
         <v>43777</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="41"/>
       <c r="B102" s="20" t="s">
         <v>57</v>
@@ -6466,7 +6473,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="41">
         <v>43800</v>
       </c>
@@ -6488,7 +6495,7 @@
         <v>43817</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="41"/>
       <c r="B104" s="20" t="s">
         <v>55</v>
@@ -6510,7 +6517,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="41"/>
       <c r="B105" s="20" t="s">
         <v>55</v>
@@ -6532,7 +6539,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="47" t="s">
         <v>45</v>
       </c>
@@ -6550,7 +6557,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="41">
         <v>43831</v>
       </c>
@@ -6572,7 +6579,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="41"/>
       <c r="B108" s="20" t="s">
         <v>71</v>
@@ -6594,7 +6601,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="41">
         <v>43891</v>
       </c>
@@ -6618,7 +6625,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="41"/>
       <c r="B110" s="20" t="s">
         <v>121</v>
@@ -6638,7 +6645,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="41"/>
       <c r="B111" s="20" t="s">
         <v>123</v>
@@ -6658,7 +6665,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="41">
         <v>43922</v>
       </c>
@@ -6682,7 +6689,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="41"/>
       <c r="B113" s="20" t="s">
         <v>47</v>
@@ -6704,7 +6711,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="41">
         <v>43952</v>
       </c>
@@ -6722,7 +6729,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="41">
         <v>43983</v>
       </c>
@@ -6740,7 +6747,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="41">
         <v>44013</v>
       </c>
@@ -6758,7 +6765,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="41">
         <v>44044</v>
       </c>
@@ -6782,7 +6789,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="41">
         <v>44075</v>
       </c>
@@ -6804,7 +6811,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="41">
         <v>44105</v>
       </c>
@@ -6822,7 +6829,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="41">
         <v>44136</v>
       </c>
@@ -6840,7 +6847,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="41">
         <v>44166</v>
       </c>
@@ -6864,7 +6871,7 @@
         <v>44173</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="41"/>
       <c r="B122" s="20" t="s">
         <v>55</v>
@@ -6886,7 +6893,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="41"/>
       <c r="B123" s="20" t="s">
         <v>71</v>
@@ -6908,7 +6915,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="47" t="s">
         <v>46</v>
       </c>
@@ -6926,7 +6933,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="41">
         <v>44197</v>
       </c>
@@ -6950,7 +6957,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="41">
         <v>44228</v>
       </c>
@@ -6972,7 +6979,7 @@
         <v>44249</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="41"/>
       <c r="B127" s="20" t="s">
         <v>53</v>
@@ -6992,7 +6999,7 @@
         <v>44215</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="41"/>
       <c r="B128" s="20" t="s">
         <v>55</v>
@@ -7014,7 +7021,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="41"/>
       <c r="B129" s="20" t="s">
         <v>71</v>
@@ -7036,7 +7043,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="41"/>
       <c r="B130" s="20" t="s">
         <v>57</v>
@@ -7058,7 +7065,7 @@
         <v>44229</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="41">
         <v>44378</v>
       </c>
@@ -7082,7 +7089,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="41"/>
       <c r="B132" s="20" t="s">
         <v>55</v>
@@ -7104,7 +7111,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="41"/>
       <c r="B133" s="20" t="s">
         <v>55</v>
@@ -7126,7 +7133,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="41">
         <v>44440</v>
       </c>
@@ -7148,7 +7155,7 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="41">
         <v>44470</v>
       </c>
@@ -7172,7 +7179,7 @@
         <v>44489</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" s="41"/>
       <c r="B136" s="20" t="s">
         <v>136</v>
@@ -7194,7 +7201,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" s="41"/>
       <c r="B137" s="20" t="s">
         <v>121</v>
@@ -7214,7 +7221,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" s="47" t="s">
         <v>52</v>
       </c>
@@ -7232,7 +7239,7 @@
       <c r="J138" s="11"/>
       <c r="K138" s="20"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" s="41">
         <v>44562</v>
       </c>
@@ -7256,7 +7263,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" s="41"/>
       <c r="B140" s="20" t="s">
         <v>57</v>
@@ -7278,7 +7285,7 @@
         <v>44589</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" s="41"/>
       <c r="B141" s="20" t="s">
         <v>55</v>
@@ -7300,7 +7307,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" s="41">
         <v>44593</v>
       </c>
@@ -7324,7 +7331,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" s="41"/>
       <c r="B143" s="20" t="s">
         <v>55</v>
@@ -7346,7 +7353,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" s="41"/>
       <c r="B144" s="20" t="s">
         <v>71</v>
@@ -7368,7 +7375,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" s="41"/>
       <c r="B145" s="20" t="s">
         <v>55</v>
@@ -7390,7 +7397,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="41">
         <v>44652</v>
       </c>
@@ -7414,7 +7421,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" s="41"/>
       <c r="B147" s="20" t="s">
         <v>57</v>
@@ -7436,7 +7443,7 @@
         <v>44680</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" s="41">
         <v>44682</v>
       </c>
@@ -7460,7 +7467,7 @@
         <v>44704</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" s="41">
         <v>44713</v>
       </c>
@@ -7482,7 +7489,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" s="41"/>
       <c r="B150" s="20" t="s">
         <v>55</v>
@@ -7504,7 +7511,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" s="41"/>
       <c r="B151" s="20" t="s">
         <v>57</v>
@@ -7526,7 +7533,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" s="41"/>
       <c r="B152" s="20" t="s">
         <v>57</v>
@@ -7548,7 +7555,7 @@
         <v>44764</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="41"/>
       <c r="B153" s="20" t="s">
         <v>55</v>
@@ -7570,7 +7577,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" s="41"/>
       <c r="B154" s="20" t="s">
         <v>55</v>
@@ -7592,7 +7599,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" s="41">
         <v>44805</v>
       </c>
@@ -7616,7 +7623,7 @@
         <v>44811</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" s="41"/>
       <c r="B156" s="20" t="s">
         <v>57</v>
@@ -7638,7 +7645,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" s="41">
         <v>44835</v>
       </c>
@@ -7662,7 +7669,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" s="41"/>
       <c r="B158" s="20" t="s">
         <v>57</v>
@@ -7684,7 +7691,7 @@
         <v>44841</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" s="41"/>
       <c r="B159" s="20" t="s">
         <v>53</v>
@@ -7704,7 +7711,7 @@
         <v>44845</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" s="41"/>
       <c r="B160" s="20" t="s">
         <v>57</v>
@@ -7726,7 +7733,7 @@
         <v>44854</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" s="41"/>
       <c r="B161" s="20" t="s">
         <v>55</v>
@@ -7748,7 +7755,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" s="41">
         <v>44866</v>
       </c>
@@ -7770,7 +7777,7 @@
         <v>44893</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" s="41"/>
       <c r="B163" s="20" t="s">
         <v>57</v>
@@ -7792,7 +7799,7 @@
         <v>44876</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" s="41"/>
       <c r="B164" s="20" t="s">
         <v>57</v>
@@ -7814,7 +7821,7 @@
         <v>44887</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" s="41">
         <v>44896</v>
       </c>
@@ -7838,7 +7845,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" s="47" t="s">
         <v>145</v>
       </c>
@@ -7856,7 +7863,7 @@
       <c r="J166" s="11"/>
       <c r="K166" s="20"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" s="41">
         <v>44986</v>
       </c>
@@ -7880,7 +7887,7 @@
         <v>44995</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" s="41">
         <v>45017</v>
       </c>
@@ -7904,7 +7911,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" s="41">
         <v>45047</v>
       </c>
@@ -7922,7 +7929,7 @@
       <c r="J169" s="11"/>
       <c r="K169" s="20"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" s="41">
         <v>45078</v>
       </c>
@@ -7946,7 +7953,7 @@
         <v>45082</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171" s="41">
         <v>45139</v>
       </c>
@@ -7970,7 +7977,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" s="41"/>
       <c r="B172" s="20" t="s">
         <v>57</v>
@@ -7992,7 +7999,7 @@
         <v>45167</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" s="41">
         <v>45170</v>
       </c>
@@ -8016,7 +8023,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174" s="41">
         <v>45200</v>
       </c>
@@ -8040,7 +8047,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175" s="41"/>
       <c r="B175" s="20" t="s">
         <v>57</v>
@@ -8062,7 +8069,7 @@
         <v>45230</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176" s="41"/>
       <c r="B176" s="20"/>
       <c r="C176" s="13"/>
@@ -8078,7 +8085,7 @@
       <c r="J176" s="11"/>
       <c r="K176" s="20"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177" s="41"/>
       <c r="B177" s="20"/>
       <c r="C177" s="13"/>
@@ -8094,7 +8101,7 @@
       <c r="J177" s="11"/>
       <c r="K177" s="20"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178" s="41"/>
       <c r="B178" s="20"/>
       <c r="C178" s="13"/>
@@ -8110,7 +8117,7 @@
       <c r="J178" s="11"/>
       <c r="K178" s="20"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179" s="41"/>
       <c r="B179" s="20"/>
       <c r="C179" s="13"/>
@@ -8126,7 +8133,7 @@
       <c r="J179" s="11"/>
       <c r="K179" s="20"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180" s="41"/>
       <c r="B180" s="20"/>
       <c r="C180" s="13"/>
@@ -8142,7 +8149,7 @@
       <c r="J180" s="11"/>
       <c r="K180" s="20"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181" s="41"/>
       <c r="B181" s="20"/>
       <c r="C181" s="13"/>
@@ -8158,7 +8165,7 @@
       <c r="J181" s="11"/>
       <c r="K181" s="20"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182" s="41"/>
       <c r="B182" s="20"/>
       <c r="C182" s="13"/>
@@ -8174,7 +8181,7 @@
       <c r="J182" s="11"/>
       <c r="K182" s="20"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A183" s="41"/>
       <c r="B183" s="20"/>
       <c r="C183" s="13"/>
@@ -8190,7 +8197,7 @@
       <c r="J183" s="11"/>
       <c r="K183" s="20"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184" s="41"/>
       <c r="B184" s="20"/>
       <c r="C184" s="13"/>
@@ -8206,7 +8213,7 @@
       <c r="J184" s="11"/>
       <c r="K184" s="20"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185" s="41"/>
       <c r="B185" s="20"/>
       <c r="C185" s="13"/>
@@ -8222,7 +8229,7 @@
       <c r="J185" s="11"/>
       <c r="K185" s="20"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186" s="41"/>
       <c r="B186" s="20"/>
       <c r="C186" s="13"/>
@@ -8238,7 +8245,7 @@
       <c r="J186" s="11"/>
       <c r="K186" s="20"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187" s="41"/>
       <c r="B187" s="20"/>
       <c r="C187" s="13"/>
@@ -8254,7 +8261,7 @@
       <c r="J187" s="11"/>
       <c r="K187" s="20"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188" s="41"/>
       <c r="B188" s="20"/>
       <c r="C188" s="13"/>
@@ -8270,7 +8277,7 @@
       <c r="J188" s="11"/>
       <c r="K188" s="20"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189" s="41"/>
       <c r="B189" s="20"/>
       <c r="C189" s="13"/>
@@ -8286,7 +8293,7 @@
       <c r="J189" s="11"/>
       <c r="K189" s="20"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A190" s="41"/>
       <c r="B190" s="20"/>
       <c r="C190" s="13"/>
@@ -8302,7 +8309,7 @@
       <c r="J190" s="11"/>
       <c r="K190" s="20"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A191" s="41"/>
       <c r="B191" s="20"/>
       <c r="C191" s="13"/>
@@ -8318,7 +8325,7 @@
       <c r="J191" s="11"/>
       <c r="K191" s="20"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A192" s="41"/>
       <c r="B192" s="20"/>
       <c r="C192" s="13"/>
@@ -8334,7 +8341,7 @@
       <c r="J192" s="11"/>
       <c r="K192" s="20"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A193" s="41"/>
       <c r="B193" s="20"/>
       <c r="C193" s="13"/>
@@ -8350,7 +8357,7 @@
       <c r="J193" s="11"/>
       <c r="K193" s="20"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A194" s="41"/>
       <c r="B194" s="20"/>
       <c r="C194" s="13"/>
@@ -8366,7 +8373,7 @@
       <c r="J194" s="11"/>
       <c r="K194" s="20"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A195" s="41"/>
       <c r="B195" s="20"/>
       <c r="C195" s="13"/>
@@ -8382,7 +8389,7 @@
       <c r="J195" s="11"/>
       <c r="K195" s="20"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A196" s="41"/>
       <c r="B196" s="20"/>
       <c r="C196" s="13"/>
@@ -8398,7 +8405,7 @@
       <c r="J196" s="11"/>
       <c r="K196" s="20"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A197" s="41"/>
       <c r="B197" s="20"/>
       <c r="C197" s="13"/>
@@ -8414,7 +8421,7 @@
       <c r="J197" s="11"/>
       <c r="K197" s="20"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A198" s="41"/>
       <c r="B198" s="20"/>
       <c r="C198" s="13"/>
@@ -8430,7 +8437,7 @@
       <c r="J198" s="11"/>
       <c r="K198" s="20"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A199" s="41"/>
       <c r="B199" s="20"/>
       <c r="C199" s="13"/>
@@ -8446,7 +8453,7 @@
       <c r="J199" s="11"/>
       <c r="K199" s="20"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A200" s="41"/>
       <c r="B200" s="20"/>
       <c r="C200" s="13"/>
@@ -8462,7 +8469,7 @@
       <c r="J200" s="11"/>
       <c r="K200" s="20"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A201" s="41"/>
       <c r="B201" s="20"/>
       <c r="C201" s="13"/>
@@ -8478,7 +8485,7 @@
       <c r="J201" s="11"/>
       <c r="K201" s="20"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A202" s="41"/>
       <c r="B202" s="20"/>
       <c r="C202" s="13"/>
@@ -8494,7 +8501,7 @@
       <c r="J202" s="11"/>
       <c r="K202" s="20"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A203" s="41"/>
       <c r="B203" s="20"/>
       <c r="C203" s="13"/>
@@ -8510,7 +8517,7 @@
       <c r="J203" s="11"/>
       <c r="K203" s="20"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A204" s="42"/>
       <c r="B204" s="15"/>
       <c r="C204" s="43"/>
@@ -8541,10 +8548,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8567,28 +8574,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="38" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="38" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -8601,7 +8608,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -8630,7 +8637,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>53.343000000000004</v>
       </c>
@@ -8662,7 +8669,7 @@
         <v>0.20799999999999974</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E4" s="1">
         <f>IF(E3=0,0,IF(ISBLANK(E3),"",VLOOKUP(E3,E7:F14,2)))</f>
         <v>0</v>
@@ -8677,10 +8684,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C6" s="39" t="s">
         <v>28</v>
       </c>
@@ -8700,7 +8707,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" s="38">
         <v>1</v>
       </c>
@@ -8726,7 +8733,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="38">
         <v>2</v>
       </c>
@@ -8752,7 +8759,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="38">
         <v>3</v>
       </c>
@@ -8778,7 +8785,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="38">
         <v>4</v>
       </c>
@@ -8804,7 +8811,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="38">
         <v>5</v>
       </c>
@@ -8830,7 +8837,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="38">
         <v>6</v>
       </c>
@@ -8856,7 +8863,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="38">
         <v>7</v>
       </c>
@@ -8882,7 +8889,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="38">
         <v>8</v>
       </c>
@@ -8908,7 +8915,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="38">
         <v>9</v>
       </c>
@@ -8928,7 +8935,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" s="38">
         <v>10</v>
       </c>
@@ -8948,7 +8955,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="38">
         <v>11</v>
       </c>
@@ -8968,7 +8975,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="38">
         <v>12</v>
       </c>
@@ -8989,7 +8996,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="38">
         <v>13</v>
       </c>
@@ -9010,7 +9017,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="38">
         <v>14</v>
       </c>
@@ -9031,7 +9038,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="38">
         <v>15</v>
       </c>
@@ -9052,7 +9059,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="38">
         <v>16</v>
       </c>
@@ -9073,7 +9080,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="38">
         <v>17</v>
       </c>
@@ -9094,7 +9101,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="38">
         <v>18</v>
       </c>
@@ -9115,7 +9122,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="38">
         <v>19</v>
       </c>
@@ -9136,7 +9143,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="38">
         <v>20</v>
       </c>
@@ -9157,7 +9164,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="38">
         <v>21</v>
       </c>
@@ -9178,7 +9185,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="38">
         <v>22</v>
       </c>
@@ -9199,7 +9206,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="38">
         <v>23</v>
       </c>
@@ -9220,7 +9227,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="38">
         <v>24</v>
       </c>
@@ -9241,7 +9248,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="38">
         <v>25</v>
       </c>
@@ -9262,7 +9269,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="38">
         <v>26</v>
       </c>
@@ -9283,7 +9290,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="38">
         <v>27</v>
       </c>
@@ -9304,7 +9311,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C34" s="38">
         <v>28</v>
       </c>
@@ -9325,7 +9332,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C35" s="38">
         <v>29</v>
       </c>
@@ -9346,7 +9353,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="38">
         <v>30</v>
       </c>
@@ -9367,7 +9374,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="38">
         <v>31</v>
       </c>
@@ -9388,7 +9395,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="38">
         <v>32</v>
       </c>
@@ -9397,7 +9404,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="38">
         <v>33</v>
       </c>
@@ -9406,7 +9413,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="38">
         <v>34</v>
       </c>
@@ -9415,7 +9422,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="38">
         <v>35</v>
       </c>
@@ -9424,7 +9431,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="38">
         <v>36</v>
       </c>
@@ -9433,7 +9440,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="38">
         <v>37</v>
       </c>
@@ -9442,7 +9449,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="38">
         <v>38</v>
       </c>
@@ -9451,7 +9458,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C45" s="38">
         <v>39</v>
       </c>
@@ -9460,7 +9467,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="38">
         <v>40</v>
       </c>
@@ -9469,7 +9476,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="38">
         <v>41</v>
       </c>
@@ -9478,7 +9485,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="38">
         <v>42</v>
       </c>
@@ -9487,7 +9494,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="38">
         <v>43</v>
       </c>
@@ -9496,7 +9503,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="38">
         <v>44</v>
       </c>
@@ -9505,7 +9512,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="38">
         <v>45</v>
       </c>
@@ -9514,7 +9521,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="38">
         <v>46</v>
       </c>
@@ -9523,7 +9530,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C53" s="38">
         <v>47</v>
       </c>
@@ -9532,7 +9539,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="38">
         <v>48</v>
       </c>
@@ -9541,7 +9548,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C55" s="38">
         <v>49</v>
       </c>
@@ -9550,7 +9557,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="38">
         <v>50</v>
       </c>
@@ -9559,7 +9566,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="38">
         <v>51</v>
       </c>
@@ -9568,7 +9575,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="38">
         <v>52</v>
       </c>
@@ -9577,7 +9584,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C59" s="38">
         <v>53</v>
       </c>
@@ -9586,7 +9593,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C60" s="38">
         <v>54</v>
       </c>
@@ -9595,7 +9602,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C61" s="38">
         <v>55</v>
       </c>
@@ -9604,7 +9611,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C62" s="38">
         <v>56</v>
       </c>
@@ -9613,7 +9620,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C63" s="38">
         <v>57</v>
       </c>
@@ -9622,7 +9629,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C64" s="38">
         <v>58</v>
       </c>
@@ -9631,7 +9638,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C65" s="38">
         <v>59</v>
       </c>
@@ -9640,7 +9647,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C66" s="38">
         <v>60</v>
       </c>
@@ -9649,7 +9656,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>

<commit_message>
Update Leave Card File 1/12/2024 4:30 pm
</commit_message>
<xml_diff>
--- a/CASUAL/LA ACCOUNTING/ABELA, IMELDA.xlsx
+++ b/CASUAL/LA ACCOUNTING/ABELA, IMELDA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA ACCOUNTING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA ACCOUNTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC45DE8-C87F-4829-BF4E-31978707C9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="2018 LEAVE CREDITS" sheetId="4" r:id="rId1"/>
@@ -27,7 +26,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="161">
   <si>
     <t>PERIOD</t>
   </si>
@@ -525,7 +524,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -903,17 +902,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -923,6 +919,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1434,7 +1433,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1451,25 +1450,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K120" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K121" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
+    <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1481,25 +1480,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K204" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K204" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1806,34 +1805,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K120"/>
+  <dimension ref="A2:K121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3696" topLeftCell="A85" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A79" activePane="bottomLeft"/>
       <selection activeCell="I9" sqref="I9"/>
-      <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
+      <selection pane="bottomLeft" activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -1845,16 +1844,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -1863,18 +1862,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>43101</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -1885,16 +1884,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -1902,7 +1901,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -1915,24 +1914,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -1967,7 +1966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -1986,12 +1985,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
-        <v>87.75</v>
+        <v>86.75</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>43</v>
       </c>
@@ -2013,7 +2012,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="41">
         <v>43101</v>
       </c>
@@ -2033,7 +2032,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>43132</v>
       </c>
@@ -2059,7 +2058,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="41">
         <v>43160</v>
       </c>
@@ -2079,7 +2078,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="41">
         <v>43191</v>
       </c>
@@ -2099,7 +2098,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="41">
         <v>43221</v>
       </c>
@@ -2119,7 +2118,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="41">
         <v>43252</v>
       </c>
@@ -2139,7 +2138,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="41">
         <v>43282</v>
       </c>
@@ -2159,7 +2158,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="41">
         <v>43313</v>
       </c>
@@ -2179,7 +2178,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="41">
         <v>43344</v>
       </c>
@@ -2199,7 +2198,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="41">
         <v>43374</v>
       </c>
@@ -2219,7 +2218,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="41">
         <v>43405</v>
       </c>
@@ -2239,7 +2238,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="41">
         <v>43435</v>
       </c>
@@ -2259,7 +2258,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
         <v>44</v>
       </c>
@@ -2277,7 +2276,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="41">
         <v>43466</v>
       </c>
@@ -2303,7 +2302,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="41">
         <v>43497</v>
       </c>
@@ -2323,7 +2322,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="41">
         <v>43525</v>
       </c>
@@ -2343,7 +2342,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="41">
         <v>43556</v>
       </c>
@@ -2363,7 +2362,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="41">
         <v>43586</v>
       </c>
@@ -2383,7 +2382,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="41">
         <v>43617</v>
       </c>
@@ -2403,7 +2402,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="41">
         <v>43647</v>
       </c>
@@ -2423,7 +2422,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="41">
         <v>43678</v>
       </c>
@@ -2443,7 +2442,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="41">
         <v>43709</v>
       </c>
@@ -2463,7 +2462,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="41">
         <v>43739</v>
       </c>
@@ -2483,7 +2482,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="41">
         <v>43770</v>
       </c>
@@ -2503,7 +2502,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="41">
         <v>43800</v>
       </c>
@@ -2523,7 +2522,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="47" t="s">
         <v>45</v>
       </c>
@@ -2541,7 +2540,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="41">
         <v>43831</v>
       </c>
@@ -2565,7 +2564,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="41">
         <v>43862</v>
       </c>
@@ -2585,7 +2584,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="41">
         <v>43891</v>
       </c>
@@ -2605,7 +2604,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="41">
         <v>43922</v>
       </c>
@@ -2625,7 +2624,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="41">
         <v>43952</v>
       </c>
@@ -2645,7 +2644,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="41">
         <v>43983</v>
       </c>
@@ -2665,7 +2664,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="41">
         <v>44013</v>
       </c>
@@ -2685,7 +2684,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="41">
         <v>44044</v>
       </c>
@@ -2705,7 +2704,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="41">
         <v>44075</v>
       </c>
@@ -2725,7 +2724,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="41">
         <v>44105</v>
       </c>
@@ -2745,7 +2744,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="41">
         <v>44136</v>
       </c>
@@ -2765,7 +2764,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="41">
         <v>44166</v>
       </c>
@@ -2785,7 +2784,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="47" t="s">
         <v>46</v>
       </c>
@@ -2803,7 +2802,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="41">
         <v>44197</v>
       </c>
@@ -2823,7 +2822,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="41">
         <v>44228</v>
       </c>
@@ -2847,7 +2846,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="41"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13">
@@ -2865,7 +2864,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="41">
         <v>44256</v>
       </c>
@@ -2885,7 +2884,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="41">
         <v>44287</v>
       </c>
@@ -2905,7 +2904,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="41">
         <v>44317</v>
       </c>
@@ -2925,7 +2924,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="41">
         <v>44348</v>
       </c>
@@ -2945,7 +2944,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="41">
         <v>44378</v>
       </c>
@@ -2965,7 +2964,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="41">
         <v>44409</v>
       </c>
@@ -2985,7 +2984,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="41">
         <v>44440</v>
       </c>
@@ -3005,7 +3004,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="41">
         <v>44470</v>
       </c>
@@ -3031,7 +3030,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="41">
         <v>44501</v>
       </c>
@@ -3051,7 +3050,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="41">
         <v>44531</v>
       </c>
@@ -3071,7 +3070,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="47" t="s">
         <v>52</v>
       </c>
@@ -3089,7 +3088,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="41">
         <v>44562</v>
       </c>
@@ -3109,7 +3108,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="41">
         <v>44593</v>
       </c>
@@ -3129,7 +3128,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="41">
         <v>44621</v>
       </c>
@@ -3153,7 +3152,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="41">
         <v>44652</v>
       </c>
@@ -3173,7 +3172,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="41"/>
       <c r="B68" s="20" t="s">
         <v>155</v>
@@ -3193,7 +3192,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="41">
         <v>44682</v>
       </c>
@@ -3217,7 +3216,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="41">
         <v>44713</v>
       </c>
@@ -3241,7 +3240,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="41">
         <v>44743</v>
       </c>
@@ -3265,7 +3264,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="41">
         <v>44774</v>
       </c>
@@ -3289,7 +3288,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="41">
         <v>44805</v>
       </c>
@@ -3313,7 +3312,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="41">
         <v>44835</v>
       </c>
@@ -3339,7 +3338,7 @@
         <v>44855</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="41"/>
       <c r="B75" s="20" t="s">
         <v>149</v>
@@ -3359,7 +3358,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="48"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="41">
         <v>44866</v>
       </c>
@@ -3385,7 +3384,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="41"/>
       <c r="B77" s="20" t="s">
         <v>62</v>
@@ -3407,7 +3406,7 @@
         <v>44894</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="41">
         <v>44896</v>
       </c>
@@ -3431,7 +3430,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="47" t="s">
         <v>145</v>
       </c>
@@ -3449,7 +3448,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="41">
         <v>44927</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="41">
         <v>44958</v>
       </c>
@@ -3495,7 +3494,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="41">
         <v>44986</v>
       </c>
@@ -3515,7 +3514,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="41">
         <v>45017</v>
       </c>
@@ -3535,7 +3534,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="41">
         <v>45047</v>
       </c>
@@ -3555,7 +3554,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="41">
         <v>45078</v>
       </c>
@@ -3575,7 +3574,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="41">
         <v>45108</v>
       </c>
@@ -3595,7 +3594,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="41">
         <v>45139</v>
       </c>
@@ -3615,7 +3614,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="48"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="41">
         <v>45170</v>
       </c>
@@ -3635,7 +3634,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="41">
         <v>45200</v>
       </c>
@@ -3661,7 +3660,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="41">
         <v>45231</v>
       </c>
@@ -3685,7 +3684,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="41">
         <v>45261</v>
       </c>
@@ -3707,7 +3706,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="41"/>
       <c r="B92" s="20" t="s">
         <v>158</v>
@@ -3729,7 +3728,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="47" t="s">
         <v>157</v>
       </c>
@@ -3747,7 +3746,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="41">
         <v>45292</v>
       </c>
@@ -3771,27 +3770,28 @@
         <v>45293</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A95" s="41">
-        <v>45323</v>
-      </c>
-      <c r="B95" s="20"/>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="41"/>
+      <c r="B95" s="20" t="s">
+        <v>57</v>
+      </c>
       <c r="C95" s="13"/>
       <c r="D95" s="40"/>
       <c r="E95" s="9"/>
       <c r="F95" s="20"/>
-      <c r="G95" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H95" s="40"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="40">
+        <v>1</v>
+      </c>
       <c r="I95" s="9"/>
       <c r="J95" s="11"/>
-      <c r="K95" s="20"/>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K95" s="48">
+        <v>45301</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="41">
-        <v>45352</v>
+        <v>45323</v>
       </c>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -3807,9 +3807,9 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="41">
-        <v>45383</v>
+        <v>45352</v>
       </c>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -3825,9 +3825,9 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="41">
-        <v>45413</v>
+        <v>45383</v>
       </c>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -3843,9 +3843,9 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="41">
-        <v>45444</v>
+        <v>45413</v>
       </c>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -3861,9 +3861,9 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="41">
-        <v>45474</v>
+        <v>45444</v>
       </c>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -3879,8 +3879,10 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A101" s="41"/>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="41">
+        <v>45474</v>
+      </c>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
       <c r="D101" s="40"/>
@@ -3895,7 +3897,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="41"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -3911,7 +3913,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="41"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -3927,7 +3929,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="41"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -3943,7 +3945,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="41"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -3959,7 +3961,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="41"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -3975,7 +3977,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="41"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -3991,7 +3993,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="41"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4007,7 +4009,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="41"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -4023,7 +4025,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="41"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -4039,7 +4041,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="41"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -4055,7 +4057,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="41"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -4071,7 +4073,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="41"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -4087,7 +4089,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="41"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -4103,7 +4105,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="41"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -4119,7 +4121,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="41"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -4135,7 +4137,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="41"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -4151,7 +4153,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="41"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -4167,7 +4169,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="41"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -4183,41 +4185,57 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A120" s="42"/>
-      <c r="B120" s="15"/>
-      <c r="C120" s="43"/>
-      <c r="D120" s="44"/>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="41"/>
+      <c r="B120" s="20"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="40"/>
       <c r="E120" s="9"/>
-      <c r="F120" s="15"/>
-      <c r="G120" s="43" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H120" s="44"/>
+      <c r="F120" s="20"/>
+      <c r="G120" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H120" s="40"/>
       <c r="I120" s="9"/>
-      <c r="J120" s="12"/>
-      <c r="K120" s="15"/>
+      <c r="J120" s="11"/>
+      <c r="K120" s="20"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" s="42"/>
+      <c r="B121" s="15"/>
+      <c r="C121" s="43"/>
+      <c r="D121" s="44"/>
+      <c r="E121" s="9"/>
+      <c r="F121" s="15"/>
+      <c r="G121" s="43" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H121" s="44"/>
+      <c r="I121" s="9"/>
+      <c r="J121" s="12"/>
+      <c r="K121" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4240,34 +4258,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K204"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3984" topLeftCell="A162" activePane="bottomLeft"/>
+      <pane ySplit="3990" topLeftCell="A162" activePane="bottomLeft"/>
       <selection activeCell="I9" sqref="I9"/>
       <selection pane="bottomLeft" activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -4279,16 +4297,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -4297,18 +4315,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>43101</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -4319,16 +4337,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -4336,7 +4354,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -4349,24 +4367,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -4401,7 +4419,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -4425,7 +4443,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>43</v>
       </c>
@@ -4447,7 +4465,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="41">
         <v>43101</v>
       </c>
@@ -4469,7 +4487,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="41"/>
       <c r="B12" s="20" t="s">
         <v>57</v>
@@ -4491,7 +4509,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="41"/>
       <c r="B13" s="20" t="s">
         <v>66</v>
@@ -4511,7 +4529,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
       <c r="B14" s="20" t="s">
         <v>55</v>
@@ -4533,7 +4551,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="41">
         <v>43132</v>
       </c>
@@ -4555,7 +4573,7 @@
         <v>43138</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="20" t="s">
         <v>57</v>
@@ -4577,7 +4595,7 @@
         <v>43133</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
       <c r="B17" s="20" t="s">
         <v>57</v>
@@ -4599,7 +4617,7 @@
         <v>43117</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>
       <c r="B18" s="20" t="s">
         <v>57</v>
@@ -4619,7 +4637,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="48"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
       <c r="B19" s="20" t="s">
         <v>57</v>
@@ -4641,7 +4659,7 @@
         <v>43146</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="41"/>
       <c r="B20" s="20" t="s">
         <v>55</v>
@@ -4663,7 +4681,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="41"/>
       <c r="B21" s="20" t="s">
         <v>57</v>
@@ -4685,7 +4703,7 @@
         <v>43159</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="41">
         <v>43160</v>
       </c>
@@ -4707,7 +4725,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
       <c r="B23" s="20" t="s">
         <v>71</v>
@@ -4729,7 +4747,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="41"/>
       <c r="B24" s="20" t="s">
         <v>55</v>
@@ -4751,7 +4769,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="41">
         <v>43191</v>
       </c>
@@ -4775,7 +4793,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="41"/>
       <c r="B26" s="20" t="s">
         <v>57</v>
@@ -4797,7 +4815,7 @@
         <v>43203</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
       <c r="B27" s="20" t="s">
         <v>55</v>
@@ -4819,7 +4837,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="41"/>
       <c r="B28" s="20" t="s">
         <v>71</v>
@@ -4841,7 +4859,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="41"/>
       <c r="B29" s="20" t="s">
         <v>75</v>
@@ -4863,7 +4881,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="41"/>
       <c r="B30" s="20" t="s">
         <v>55</v>
@@ -4885,7 +4903,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="41">
         <v>43221</v>
       </c>
@@ -4909,7 +4927,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="41"/>
       <c r="B32" s="15" t="s">
         <v>71</v>
@@ -4931,7 +4949,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="41"/>
       <c r="B33" s="15" t="s">
         <v>71</v>
@@ -4953,7 +4971,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="41"/>
       <c r="B34" s="15" t="s">
         <v>84</v>
@@ -4973,7 +4991,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="15"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="41">
         <v>43252</v>
       </c>
@@ -4997,7 +5015,7 @@
         <v>43258</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="41"/>
       <c r="B36" s="15" t="s">
         <v>57</v>
@@ -5019,7 +5037,7 @@
         <v>43270</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="41"/>
       <c r="B37" s="15" t="s">
         <v>57</v>
@@ -5041,7 +5059,7 @@
         <v>43276</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="41"/>
       <c r="B38" s="15" t="s">
         <v>85</v>
@@ -5061,7 +5079,7 @@
       <c r="J38" s="12"/>
       <c r="K38" s="49"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="41">
         <v>43282</v>
       </c>
@@ -5085,7 +5103,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="41"/>
       <c r="B40" s="20" t="s">
         <v>57</v>
@@ -5105,7 +5123,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="41"/>
       <c r="B41" s="20" t="s">
         <v>87</v>
@@ -5125,7 +5143,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="41">
         <v>43313</v>
       </c>
@@ -5149,7 +5167,7 @@
         <v>43318</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="41"/>
       <c r="B43" s="20" t="s">
         <v>57</v>
@@ -5171,7 +5189,7 @@
         <v>43325</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="41"/>
       <c r="B44" s="20" t="s">
         <v>57</v>
@@ -5193,7 +5211,7 @@
         <v>43328</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="41"/>
       <c r="B45" s="20" t="s">
         <v>88</v>
@@ -5213,7 +5231,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="48"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="41">
         <v>43344</v>
       </c>
@@ -5237,7 +5255,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="41"/>
       <c r="B47" s="20" t="s">
         <v>55</v>
@@ -5259,7 +5277,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="41"/>
       <c r="B48" s="20" t="s">
         <v>90</v>
@@ -5277,7 +5295,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="48"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="41">
         <v>43374</v>
       </c>
@@ -5301,7 +5319,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="41"/>
       <c r="B50" s="20" t="s">
         <v>75</v>
@@ -5323,7 +5341,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="41"/>
       <c r="B51" s="20" t="s">
         <v>93</v>
@@ -5343,7 +5361,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="41">
         <v>43405</v>
       </c>
@@ -5367,7 +5385,7 @@
         <v>43425</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="41"/>
       <c r="B53" s="20" t="s">
         <v>55</v>
@@ -5389,7 +5407,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="41"/>
       <c r="B54" s="20" t="s">
         <v>95</v>
@@ -5407,7 +5425,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="48"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="41">
         <v>43435</v>
       </c>
@@ -5431,7 +5449,7 @@
         <v>43452</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="41"/>
       <c r="B56" s="20" t="s">
         <v>57</v>
@@ -5453,7 +5471,7 @@
         <v>43445</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="41"/>
       <c r="B57" s="20" t="s">
         <v>55</v>
@@ -5475,7 +5493,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="41"/>
       <c r="B58" s="20" t="s">
         <v>97</v>
@@ -5493,7 +5511,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="48"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="47" t="s">
         <v>44</v>
       </c>
@@ -5511,7 +5529,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="41">
         <v>43466</v>
       </c>
@@ -5533,7 +5551,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="41"/>
       <c r="B61" s="20" t="s">
         <v>71</v>
@@ -5555,7 +5573,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="41">
         <v>43497</v>
       </c>
@@ -5579,7 +5597,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="41"/>
       <c r="B63" s="20" t="s">
         <v>57</v>
@@ -5601,7 +5619,7 @@
         <v>43517</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="41"/>
       <c r="B64" s="20" t="s">
         <v>53</v>
@@ -5621,7 +5639,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="41"/>
       <c r="B65" s="20" t="s">
         <v>55</v>
@@ -5643,7 +5661,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="41">
         <v>43525</v>
       </c>
@@ -5667,7 +5685,7 @@
         <v>43531</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="41"/>
       <c r="B67" s="20" t="s">
         <v>71</v>
@@ -5689,7 +5707,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="41"/>
       <c r="B68" s="20" t="s">
         <v>57</v>
@@ -5711,7 +5729,7 @@
         <v>43552</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="41">
         <v>43556</v>
       </c>
@@ -5735,7 +5753,7 @@
         <v>43817</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="41"/>
       <c r="B70" s="20" t="s">
         <v>57</v>
@@ -5757,7 +5775,7 @@
         <v>43557</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="41"/>
       <c r="B71" s="20" t="s">
         <v>57</v>
@@ -5779,7 +5797,7 @@
         <v>43572</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="41"/>
       <c r="B72" s="20" t="s">
         <v>55</v>
@@ -5801,7 +5819,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="41">
         <v>43586</v>
       </c>
@@ -5825,7 +5843,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="41"/>
       <c r="B74" s="20" t="s">
         <v>75</v>
@@ -5847,7 +5865,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="41"/>
       <c r="B75" s="20" t="s">
         <v>57</v>
@@ -5869,7 +5887,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="41"/>
       <c r="B76" s="20" t="s">
         <v>57</v>
@@ -5891,7 +5909,7 @@
         <v>43601</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="41"/>
       <c r="B77" s="20" t="s">
         <v>55</v>
@@ -5913,7 +5931,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="41"/>
       <c r="B78" s="20" t="s">
         <v>57</v>
@@ -5935,7 +5953,7 @@
         <v>43615</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="41">
         <v>43617</v>
       </c>
@@ -5959,7 +5977,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="41"/>
       <c r="B80" s="20" t="s">
         <v>71</v>
@@ -5981,7 +5999,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="41"/>
       <c r="B81" s="20" t="s">
         <v>57</v>
@@ -6003,7 +6021,7 @@
         <v>43629</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="41"/>
       <c r="B82" s="20" t="s">
         <v>57</v>
@@ -6025,7 +6043,7 @@
         <v>43633</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="41"/>
       <c r="B83" s="20" t="s">
         <v>108</v>
@@ -6047,7 +6065,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="41"/>
       <c r="B84" s="20" t="s">
         <v>66</v>
@@ -6067,7 +6085,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="41">
         <v>43647</v>
       </c>
@@ -6091,7 +6109,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="41"/>
       <c r="B86" s="20" t="s">
         <v>57</v>
@@ -6113,7 +6131,7 @@
         <v>43663</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="41"/>
       <c r="B87" s="20" t="s">
         <v>57</v>
@@ -6135,7 +6153,7 @@
         <v>43668</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="41">
         <v>43678</v>
       </c>
@@ -6159,7 +6177,7 @@
         <v>43678</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="41"/>
       <c r="B89" s="20" t="s">
         <v>57</v>
@@ -6181,7 +6199,7 @@
         <v>43685</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="41"/>
       <c r="B90" s="20" t="s">
         <v>57</v>
@@ -6203,7 +6221,7 @@
         <v>43700</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="41"/>
       <c r="B91" s="20" t="s">
         <v>55</v>
@@ -6225,7 +6243,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="41">
         <v>43709</v>
       </c>
@@ -6249,7 +6267,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="41"/>
       <c r="B93" s="20" t="s">
         <v>55</v>
@@ -6271,7 +6289,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="41"/>
       <c r="B94" s="20" t="s">
         <v>55</v>
@@ -6293,7 +6311,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="41">
         <v>43739</v>
       </c>
@@ -6317,7 +6335,7 @@
         <v>43749</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="41"/>
       <c r="B96" s="20" t="s">
         <v>55</v>
@@ -6339,7 +6357,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="41"/>
       <c r="B97" s="20" t="s">
         <v>57</v>
@@ -6361,7 +6379,7 @@
         <v>43755</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="41"/>
       <c r="B98" s="20" t="s">
         <v>57</v>
@@ -6383,7 +6401,7 @@
         <v>43762</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="41"/>
       <c r="B99" s="20" t="s">
         <v>57</v>
@@ -6405,7 +6423,7 @@
         <v>43769</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="41">
         <v>43770</v>
       </c>
@@ -6429,7 +6447,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="41"/>
       <c r="B101" s="20" t="s">
         <v>57</v>
@@ -6451,7 +6469,7 @@
         <v>43777</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="41"/>
       <c r="B102" s="20" t="s">
         <v>57</v>
@@ -6473,7 +6491,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="41">
         <v>43800</v>
       </c>
@@ -6495,7 +6513,7 @@
         <v>43817</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="41"/>
       <c r="B104" s="20" t="s">
         <v>55</v>
@@ -6517,7 +6535,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="41"/>
       <c r="B105" s="20" t="s">
         <v>55</v>
@@ -6539,7 +6557,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="47" t="s">
         <v>45</v>
       </c>
@@ -6557,7 +6575,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="41">
         <v>43831</v>
       </c>
@@ -6579,7 +6597,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="41"/>
       <c r="B108" s="20" t="s">
         <v>71</v>
@@ -6601,7 +6619,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="41">
         <v>43891</v>
       </c>
@@ -6625,7 +6643,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="41"/>
       <c r="B110" s="20" t="s">
         <v>121</v>
@@ -6645,7 +6663,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="41"/>
       <c r="B111" s="20" t="s">
         <v>123</v>
@@ -6665,7 +6683,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="41">
         <v>43922</v>
       </c>
@@ -6689,7 +6707,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="41"/>
       <c r="B113" s="20" t="s">
         <v>47</v>
@@ -6711,7 +6729,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="41">
         <v>43952</v>
       </c>
@@ -6729,7 +6747,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="41">
         <v>43983</v>
       </c>
@@ -6747,7 +6765,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="41">
         <v>44013</v>
       </c>
@@ -6765,7 +6783,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="41">
         <v>44044</v>
       </c>
@@ -6789,7 +6807,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="41">
         <v>44075</v>
       </c>
@@ -6811,7 +6829,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="41">
         <v>44105</v>
       </c>
@@ -6829,7 +6847,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="41">
         <v>44136</v>
       </c>
@@ -6847,7 +6865,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="41">
         <v>44166</v>
       </c>
@@ -6871,7 +6889,7 @@
         <v>44173</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="41"/>
       <c r="B122" s="20" t="s">
         <v>55</v>
@@ -6893,7 +6911,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="41"/>
       <c r="B123" s="20" t="s">
         <v>71</v>
@@ -6915,7 +6933,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="47" t="s">
         <v>46</v>
       </c>
@@ -6933,7 +6951,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="41">
         <v>44197</v>
       </c>
@@ -6957,7 +6975,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="41">
         <v>44228</v>
       </c>
@@ -6979,7 +6997,7 @@
         <v>44249</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="41"/>
       <c r="B127" s="20" t="s">
         <v>53</v>
@@ -6999,7 +7017,7 @@
         <v>44215</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="41"/>
       <c r="B128" s="20" t="s">
         <v>55</v>
@@ -7021,7 +7039,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="41"/>
       <c r="B129" s="20" t="s">
         <v>71</v>
@@ -7043,7 +7061,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="41"/>
       <c r="B130" s="20" t="s">
         <v>57</v>
@@ -7065,7 +7083,7 @@
         <v>44229</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="41">
         <v>44378</v>
       </c>
@@ -7089,7 +7107,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="41"/>
       <c r="B132" s="20" t="s">
         <v>55</v>
@@ -7111,7 +7129,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="41"/>
       <c r="B133" s="20" t="s">
         <v>55</v>
@@ -7133,7 +7151,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="41">
         <v>44440</v>
       </c>
@@ -7155,7 +7173,7 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="41">
         <v>44470</v>
       </c>
@@ -7179,7 +7197,7 @@
         <v>44489</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="41"/>
       <c r="B136" s="20" t="s">
         <v>136</v>
@@ -7201,7 +7219,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="41"/>
       <c r="B137" s="20" t="s">
         <v>121</v>
@@ -7221,7 +7239,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="47" t="s">
         <v>52</v>
       </c>
@@ -7239,7 +7257,7 @@
       <c r="J138" s="11"/>
       <c r="K138" s="20"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="41">
         <v>44562</v>
       </c>
@@ -7263,7 +7281,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="41"/>
       <c r="B140" s="20" t="s">
         <v>57</v>
@@ -7285,7 +7303,7 @@
         <v>44589</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="41"/>
       <c r="B141" s="20" t="s">
         <v>55</v>
@@ -7307,7 +7325,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="41">
         <v>44593</v>
       </c>
@@ -7331,7 +7349,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="41"/>
       <c r="B143" s="20" t="s">
         <v>55</v>
@@ -7353,7 +7371,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="41"/>
       <c r="B144" s="20" t="s">
         <v>71</v>
@@ -7375,7 +7393,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="41"/>
       <c r="B145" s="20" t="s">
         <v>55</v>
@@ -7397,7 +7415,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="41">
         <v>44652</v>
       </c>
@@ -7421,7 +7439,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="41"/>
       <c r="B147" s="20" t="s">
         <v>57</v>
@@ -7443,7 +7461,7 @@
         <v>44680</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="41">
         <v>44682</v>
       </c>
@@ -7467,7 +7485,7 @@
         <v>44704</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="41">
         <v>44713</v>
       </c>
@@ -7489,7 +7507,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="41"/>
       <c r="B150" s="20" t="s">
         <v>55</v>
@@ -7511,7 +7529,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="41"/>
       <c r="B151" s="20" t="s">
         <v>57</v>
@@ -7533,7 +7551,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="41"/>
       <c r="B152" s="20" t="s">
         <v>57</v>
@@ -7555,7 +7573,7 @@
         <v>44764</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="41"/>
       <c r="B153" s="20" t="s">
         <v>55</v>
@@ -7577,7 +7595,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="41"/>
       <c r="B154" s="20" t="s">
         <v>55</v>
@@ -7599,7 +7617,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="41">
         <v>44805</v>
       </c>
@@ -7623,7 +7641,7 @@
         <v>44811</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="41"/>
       <c r="B156" s="20" t="s">
         <v>57</v>
@@ -7645,7 +7663,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="41">
         <v>44835</v>
       </c>
@@ -7669,7 +7687,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="41"/>
       <c r="B158" s="20" t="s">
         <v>57</v>
@@ -7691,7 +7709,7 @@
         <v>44841</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="41"/>
       <c r="B159" s="20" t="s">
         <v>53</v>
@@ -7711,7 +7729,7 @@
         <v>44845</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="41"/>
       <c r="B160" s="20" t="s">
         <v>57</v>
@@ -7733,7 +7751,7 @@
         <v>44854</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="41"/>
       <c r="B161" s="20" t="s">
         <v>55</v>
@@ -7755,7 +7773,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="41">
         <v>44866</v>
       </c>
@@ -7777,7 +7795,7 @@
         <v>44893</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="41"/>
       <c r="B163" s="20" t="s">
         <v>57</v>
@@ -7799,7 +7817,7 @@
         <v>44876</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="41"/>
       <c r="B164" s="20" t="s">
         <v>57</v>
@@ -7821,7 +7839,7 @@
         <v>44887</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="41">
         <v>44896</v>
       </c>
@@ -7845,7 +7863,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="47" t="s">
         <v>145</v>
       </c>
@@ -7863,7 +7881,7 @@
       <c r="J166" s="11"/>
       <c r="K166" s="20"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="41">
         <v>44986</v>
       </c>
@@ -7887,7 +7905,7 @@
         <v>44995</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="41">
         <v>45017</v>
       </c>
@@ -7911,7 +7929,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="41">
         <v>45047</v>
       </c>
@@ -7929,7 +7947,7 @@
       <c r="J169" s="11"/>
       <c r="K169" s="20"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="41">
         <v>45078</v>
       </c>
@@ -7953,7 +7971,7 @@
         <v>45082</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="41">
         <v>45139</v>
       </c>
@@ -7977,7 +7995,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="41"/>
       <c r="B172" s="20" t="s">
         <v>57</v>
@@ -7999,7 +8017,7 @@
         <v>45167</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="41">
         <v>45170</v>
       </c>
@@ -8023,7 +8041,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="41">
         <v>45200</v>
       </c>
@@ -8047,7 +8065,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="41"/>
       <c r="B175" s="20" t="s">
         <v>57</v>
@@ -8069,7 +8087,7 @@
         <v>45230</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="41"/>
       <c r="B176" s="20"/>
       <c r="C176" s="13"/>
@@ -8085,7 +8103,7 @@
       <c r="J176" s="11"/>
       <c r="K176" s="20"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="41"/>
       <c r="B177" s="20"/>
       <c r="C177" s="13"/>
@@ -8101,7 +8119,7 @@
       <c r="J177" s="11"/>
       <c r="K177" s="20"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="41"/>
       <c r="B178" s="20"/>
       <c r="C178" s="13"/>
@@ -8117,7 +8135,7 @@
       <c r="J178" s="11"/>
       <c r="K178" s="20"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="41"/>
       <c r="B179" s="20"/>
       <c r="C179" s="13"/>
@@ -8133,7 +8151,7 @@
       <c r="J179" s="11"/>
       <c r="K179" s="20"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="41"/>
       <c r="B180" s="20"/>
       <c r="C180" s="13"/>
@@ -8149,7 +8167,7 @@
       <c r="J180" s="11"/>
       <c r="K180" s="20"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="41"/>
       <c r="B181" s="20"/>
       <c r="C181" s="13"/>
@@ -8165,7 +8183,7 @@
       <c r="J181" s="11"/>
       <c r="K181" s="20"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="41"/>
       <c r="B182" s="20"/>
       <c r="C182" s="13"/>
@@ -8181,7 +8199,7 @@
       <c r="J182" s="11"/>
       <c r="K182" s="20"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="41"/>
       <c r="B183" s="20"/>
       <c r="C183" s="13"/>
@@ -8197,7 +8215,7 @@
       <c r="J183" s="11"/>
       <c r="K183" s="20"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="41"/>
       <c r="B184" s="20"/>
       <c r="C184" s="13"/>
@@ -8213,7 +8231,7 @@
       <c r="J184" s="11"/>
       <c r="K184" s="20"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="41"/>
       <c r="B185" s="20"/>
       <c r="C185" s="13"/>
@@ -8229,7 +8247,7 @@
       <c r="J185" s="11"/>
       <c r="K185" s="20"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="41"/>
       <c r="B186" s="20"/>
       <c r="C186" s="13"/>
@@ -8245,7 +8263,7 @@
       <c r="J186" s="11"/>
       <c r="K186" s="20"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="41"/>
       <c r="B187" s="20"/>
       <c r="C187" s="13"/>
@@ -8261,7 +8279,7 @@
       <c r="J187" s="11"/>
       <c r="K187" s="20"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="41"/>
       <c r="B188" s="20"/>
       <c r="C188" s="13"/>
@@ -8277,7 +8295,7 @@
       <c r="J188" s="11"/>
       <c r="K188" s="20"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="41"/>
       <c r="B189" s="20"/>
       <c r="C189" s="13"/>
@@ -8293,7 +8311,7 @@
       <c r="J189" s="11"/>
       <c r="K189" s="20"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="41"/>
       <c r="B190" s="20"/>
       <c r="C190" s="13"/>
@@ -8309,7 +8327,7 @@
       <c r="J190" s="11"/>
       <c r="K190" s="20"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="41"/>
       <c r="B191" s="20"/>
       <c r="C191" s="13"/>
@@ -8325,7 +8343,7 @@
       <c r="J191" s="11"/>
       <c r="K191" s="20"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="41"/>
       <c r="B192" s="20"/>
       <c r="C192" s="13"/>
@@ -8341,7 +8359,7 @@
       <c r="J192" s="11"/>
       <c r="K192" s="20"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="41"/>
       <c r="B193" s="20"/>
       <c r="C193" s="13"/>
@@ -8357,7 +8375,7 @@
       <c r="J193" s="11"/>
       <c r="K193" s="20"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="41"/>
       <c r="B194" s="20"/>
       <c r="C194" s="13"/>
@@ -8373,7 +8391,7 @@
       <c r="J194" s="11"/>
       <c r="K194" s="20"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="41"/>
       <c r="B195" s="20"/>
       <c r="C195" s="13"/>
@@ -8389,7 +8407,7 @@
       <c r="J195" s="11"/>
       <c r="K195" s="20"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="41"/>
       <c r="B196" s="20"/>
       <c r="C196" s="13"/>
@@ -8405,7 +8423,7 @@
       <c r="J196" s="11"/>
       <c r="K196" s="20"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="41"/>
       <c r="B197" s="20"/>
       <c r="C197" s="13"/>
@@ -8421,7 +8439,7 @@
       <c r="J197" s="11"/>
       <c r="K197" s="20"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="41"/>
       <c r="B198" s="20"/>
       <c r="C198" s="13"/>
@@ -8437,7 +8455,7 @@
       <c r="J198" s="11"/>
       <c r="K198" s="20"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="41"/>
       <c r="B199" s="20"/>
       <c r="C199" s="13"/>
@@ -8453,7 +8471,7 @@
       <c r="J199" s="11"/>
       <c r="K199" s="20"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="41"/>
       <c r="B200" s="20"/>
       <c r="C200" s="13"/>
@@ -8469,7 +8487,7 @@
       <c r="J200" s="11"/>
       <c r="K200" s="20"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="41"/>
       <c r="B201" s="20"/>
       <c r="C201" s="13"/>
@@ -8485,7 +8503,7 @@
       <c r="J201" s="11"/>
       <c r="K201" s="20"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="41"/>
       <c r="B202" s="20"/>
       <c r="C202" s="13"/>
@@ -8501,7 +8519,7 @@
       <c r="J202" s="11"/>
       <c r="K202" s="20"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="41"/>
       <c r="B203" s="20"/>
       <c r="C203" s="13"/>
@@ -8517,7 +8535,7 @@
       <c r="J203" s="11"/>
       <c r="K203" s="20"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="42"/>
       <c r="B204" s="15"/>
       <c r="C204" s="43"/>
@@ -8548,10 +8566,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8574,28 +8592,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="38" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="38" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -8608,7 +8626,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -8637,7 +8655,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>53.343000000000004</v>
       </c>
@@ -8669,7 +8687,7 @@
         <v>0.20799999999999974</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E4" s="1">
         <f>IF(E3=0,0,IF(ISBLANK(E3),"",VLOOKUP(E3,E7:F14,2)))</f>
         <v>0</v>
@@ -8684,10 +8702,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="39" t="s">
         <v>28</v>
       </c>
@@ -8707,7 +8725,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="38">
         <v>1</v>
       </c>
@@ -8733,7 +8751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="38">
         <v>2</v>
       </c>
@@ -8759,7 +8777,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="38">
         <v>3</v>
       </c>
@@ -8785,7 +8803,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="38">
         <v>4</v>
       </c>
@@ -8811,7 +8829,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="38">
         <v>5</v>
       </c>
@@ -8837,7 +8855,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="38">
         <v>6</v>
       </c>
@@ -8863,7 +8881,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="38">
         <v>7</v>
       </c>
@@ -8889,7 +8907,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="38">
         <v>8</v>
       </c>
@@ -8915,7 +8933,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="38">
         <v>9</v>
       </c>
@@ -8935,7 +8953,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="38">
         <v>10</v>
       </c>
@@ -8955,7 +8973,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="38">
         <v>11</v>
       </c>
@@ -8975,7 +8993,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="38">
         <v>12</v>
       </c>
@@ -8996,7 +9014,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="38">
         <v>13</v>
       </c>
@@ -9017,7 +9035,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="38">
         <v>14</v>
       </c>
@@ -9038,7 +9056,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="38">
         <v>15</v>
       </c>
@@ -9059,7 +9077,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="38">
         <v>16</v>
       </c>
@@ -9080,7 +9098,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="38">
         <v>17</v>
       </c>
@@ -9101,7 +9119,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="38">
         <v>18</v>
       </c>
@@ -9122,7 +9140,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="38">
         <v>19</v>
       </c>
@@ -9143,7 +9161,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="38">
         <v>20</v>
       </c>
@@ -9164,7 +9182,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="38">
         <v>21</v>
       </c>
@@ -9185,7 +9203,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="38">
         <v>22</v>
       </c>
@@ -9206,7 +9224,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="38">
         <v>23</v>
       </c>
@@ -9227,7 +9245,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="38">
         <v>24</v>
       </c>
@@ -9248,7 +9266,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="38">
         <v>25</v>
       </c>
@@ -9269,7 +9287,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="38">
         <v>26</v>
       </c>
@@ -9290,7 +9308,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="38">
         <v>27</v>
       </c>
@@ -9311,7 +9329,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="38">
         <v>28</v>
       </c>
@@ -9332,7 +9350,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="38">
         <v>29</v>
       </c>
@@ -9353,7 +9371,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="38">
         <v>30</v>
       </c>
@@ -9374,7 +9392,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="38">
         <v>31</v>
       </c>
@@ -9395,7 +9413,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="38">
         <v>32</v>
       </c>
@@ -9404,7 +9422,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="38">
         <v>33</v>
       </c>
@@ -9413,7 +9431,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="38">
         <v>34</v>
       </c>
@@ -9422,7 +9440,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="38">
         <v>35</v>
       </c>
@@ -9431,7 +9449,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="38">
         <v>36</v>
       </c>
@@ -9440,7 +9458,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="38">
         <v>37</v>
       </c>
@@ -9449,7 +9467,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="38">
         <v>38</v>
       </c>
@@ -9458,7 +9476,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="38">
         <v>39</v>
       </c>
@@ -9467,7 +9485,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="38">
         <v>40</v>
       </c>
@@ -9476,7 +9494,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="38">
         <v>41</v>
       </c>
@@ -9485,7 +9503,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="38">
         <v>42</v>
       </c>
@@ -9494,7 +9512,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="38">
         <v>43</v>
       </c>
@@ -9503,7 +9521,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="38">
         <v>44</v>
       </c>
@@ -9512,7 +9530,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="38">
         <v>45</v>
       </c>
@@ -9521,7 +9539,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="38">
         <v>46</v>
       </c>
@@ -9530,7 +9548,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="38">
         <v>47</v>
       </c>
@@ -9539,7 +9557,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="38">
         <v>48</v>
       </c>
@@ -9548,7 +9566,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="38">
         <v>49</v>
       </c>
@@ -9557,7 +9575,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="38">
         <v>50</v>
       </c>
@@ -9566,7 +9584,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="38">
         <v>51</v>
       </c>
@@ -9575,7 +9593,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="38">
         <v>52</v>
       </c>
@@ -9584,7 +9602,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="38">
         <v>53</v>
       </c>
@@ -9593,7 +9611,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="38">
         <v>54</v>
       </c>
@@ -9602,7 +9620,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="38">
         <v>55</v>
       </c>
@@ -9611,7 +9629,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="38">
         <v>56</v>
       </c>
@@ -9620,7 +9638,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="38">
         <v>57</v>
       </c>
@@ -9629,7 +9647,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="38">
         <v>58</v>
       </c>
@@ -9638,7 +9656,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="38">
         <v>59</v>
       </c>
@@ -9647,7 +9665,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="38">
         <v>60</v>
       </c>
@@ -9656,7 +9674,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>

<commit_message>
Update Leave Card 2/1/2024 4:41 PM
</commit_message>
<xml_diff>
--- a/CASUAL/LA ACCOUNTING/ABELA, IMELDA.xlsx
+++ b/CASUAL/LA ACCOUNTING/ABELA, IMELDA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA ACCOUNTING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA ACCOUNTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B87C427-E5A3-4CA5-8E6F-6DF09D147856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018 LEAVE CREDITS" sheetId="4" r:id="rId1"/>
@@ -26,7 +27,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="161">
   <si>
     <t>PERIOD</t>
   </si>
@@ -524,7 +525,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -902,14 +903,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -919,9 +923,6 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1433,7 +1434,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1450,25 +1451,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K121" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K121" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="23"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="22"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="20"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1480,25 +1481,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K204" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K204" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1805,34 +1806,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A79" activePane="bottomLeft"/>
+      <pane ySplit="3696" topLeftCell="A88" activePane="bottomLeft"/>
       <selection activeCell="I9" sqref="I9"/>
-      <selection pane="bottomLeft" activeCell="F93" sqref="F93"/>
+      <selection pane="bottomLeft" activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -1844,16 +1845,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -1862,18 +1863,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="55">
         <v>43101</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -1884,16 +1885,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -1901,7 +1902,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -1914,24 +1915,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -1966,7 +1967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -1975,7 +1976,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
-        <v>40.5</v>
+        <v>43</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -1985,12 +1986,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
-        <v>86.75</v>
+        <v>89.25</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>43</v>
       </c>
@@ -2012,7 +2013,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="41">
         <v>43101</v>
       </c>
@@ -2032,7 +2033,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="41">
         <v>43132</v>
       </c>
@@ -2058,7 +2059,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="41">
         <v>43160</v>
       </c>
@@ -2078,7 +2079,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="41">
         <v>43191</v>
       </c>
@@ -2098,7 +2099,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="41">
         <v>43221</v>
       </c>
@@ -2118,7 +2119,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="41">
         <v>43252</v>
       </c>
@@ -2138,7 +2139,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="41">
         <v>43282</v>
       </c>
@@ -2158,7 +2159,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="41">
         <v>43313</v>
       </c>
@@ -2178,7 +2179,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="41">
         <v>43344</v>
       </c>
@@ -2198,7 +2199,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="41">
         <v>43374</v>
       </c>
@@ -2218,7 +2219,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="41">
         <v>43405</v>
       </c>
@@ -2238,7 +2239,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="41">
         <v>43435</v>
       </c>
@@ -2258,7 +2259,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="47" t="s">
         <v>44</v>
       </c>
@@ -2276,7 +2277,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="41">
         <v>43466</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="41">
         <v>43497</v>
       </c>
@@ -2322,7 +2323,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="41">
         <v>43525</v>
       </c>
@@ -2342,7 +2343,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="41">
         <v>43556</v>
       </c>
@@ -2362,7 +2363,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="41">
         <v>43586</v>
       </c>
@@ -2382,7 +2383,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="41">
         <v>43617</v>
       </c>
@@ -2402,7 +2403,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="41">
         <v>43647</v>
       </c>
@@ -2422,7 +2423,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="41">
         <v>43678</v>
       </c>
@@ -2442,7 +2443,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="41">
         <v>43709</v>
       </c>
@@ -2462,7 +2463,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="41">
         <v>43739</v>
       </c>
@@ -2482,7 +2483,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="41">
         <v>43770</v>
       </c>
@@ -2502,7 +2503,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="41">
         <v>43800</v>
       </c>
@@ -2522,7 +2523,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="47" t="s">
         <v>45</v>
       </c>
@@ -2540,7 +2541,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="41">
         <v>43831</v>
       </c>
@@ -2564,7 +2565,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="41">
         <v>43862</v>
       </c>
@@ -2584,7 +2585,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="41">
         <v>43891</v>
       </c>
@@ -2604,7 +2605,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="41">
         <v>43922</v>
       </c>
@@ -2624,7 +2625,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="41">
         <v>43952</v>
       </c>
@@ -2644,7 +2645,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="41">
         <v>43983</v>
       </c>
@@ -2664,7 +2665,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="41">
         <v>44013</v>
       </c>
@@ -2684,7 +2685,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="41">
         <v>44044</v>
       </c>
@@ -2704,7 +2705,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="41">
         <v>44075</v>
       </c>
@@ -2724,7 +2725,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="41">
         <v>44105</v>
       </c>
@@ -2744,7 +2745,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="41">
         <v>44136</v>
       </c>
@@ -2764,7 +2765,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="41">
         <v>44166</v>
       </c>
@@ -2784,7 +2785,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="47" t="s">
         <v>46</v>
       </c>
@@ -2802,7 +2803,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="41">
         <v>44197</v>
       </c>
@@ -2822,7 +2823,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="41">
         <v>44228</v>
       </c>
@@ -2846,7 +2847,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="41"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13">
@@ -2864,7 +2865,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="41">
         <v>44256</v>
       </c>
@@ -2884,7 +2885,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="41">
         <v>44287</v>
       </c>
@@ -2904,7 +2905,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="41">
         <v>44317</v>
       </c>
@@ -2924,7 +2925,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="41">
         <v>44348</v>
       </c>
@@ -2944,7 +2945,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="41">
         <v>44378</v>
       </c>
@@ -2964,7 +2965,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="41">
         <v>44409</v>
       </c>
@@ -2984,7 +2985,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="41">
         <v>44440</v>
       </c>
@@ -3004,7 +3005,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="41">
         <v>44470</v>
       </c>
@@ -3030,7 +3031,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="41">
         <v>44501</v>
       </c>
@@ -3050,7 +3051,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="41">
         <v>44531</v>
       </c>
@@ -3070,7 +3071,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="47" t="s">
         <v>52</v>
       </c>
@@ -3088,7 +3089,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="41">
         <v>44562</v>
       </c>
@@ -3108,7 +3109,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="41">
         <v>44593</v>
       </c>
@@ -3128,7 +3129,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="41">
         <v>44621</v>
       </c>
@@ -3152,7 +3153,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="41">
         <v>44652</v>
       </c>
@@ -3172,7 +3173,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="41"/>
       <c r="B68" s="20" t="s">
         <v>155</v>
@@ -3192,7 +3193,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="41">
         <v>44682</v>
       </c>
@@ -3216,7 +3217,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="41">
         <v>44713</v>
       </c>
@@ -3240,7 +3241,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="41">
         <v>44743</v>
       </c>
@@ -3264,7 +3265,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="41">
         <v>44774</v>
       </c>
@@ -3288,7 +3289,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="41">
         <v>44805</v>
       </c>
@@ -3312,7 +3313,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="41">
         <v>44835</v>
       </c>
@@ -3338,7 +3339,7 @@
         <v>44855</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="41"/>
       <c r="B75" s="20" t="s">
         <v>149</v>
@@ -3358,7 +3359,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="48"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="41">
         <v>44866</v>
       </c>
@@ -3384,7 +3385,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="41"/>
       <c r="B77" s="20" t="s">
         <v>62</v>
@@ -3406,7 +3407,7 @@
         <v>44894</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="41">
         <v>44896</v>
       </c>
@@ -3430,7 +3431,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="47" t="s">
         <v>145</v>
       </c>
@@ -3448,7 +3449,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="41">
         <v>44927</v>
       </c>
@@ -3474,7 +3475,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="41">
         <v>44958</v>
       </c>
@@ -3494,7 +3495,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="41">
         <v>44986</v>
       </c>
@@ -3514,7 +3515,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="41">
         <v>45017</v>
       </c>
@@ -3534,7 +3535,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="41">
         <v>45047</v>
       </c>
@@ -3554,7 +3555,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="41">
         <v>45078</v>
       </c>
@@ -3574,7 +3575,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="41">
         <v>45108</v>
       </c>
@@ -3594,7 +3595,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="41">
         <v>45139</v>
       </c>
@@ -3614,7 +3615,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="48"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="41">
         <v>45170</v>
       </c>
@@ -3634,7 +3635,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="41">
         <v>45200</v>
       </c>
@@ -3660,7 +3661,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="41">
         <v>45231</v>
       </c>
@@ -3684,20 +3685,22 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="41">
         <v>45261</v>
       </c>
       <c r="B91" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C91" s="13"/>
+      <c r="C91" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D91" s="40"/>
       <c r="E91" s="9"/>
       <c r="F91" s="20"/>
-      <c r="G91" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G91" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H91" s="40"/>
       <c r="I91" s="9"/>
@@ -3706,7 +3709,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="41"/>
       <c r="B92" s="20" t="s">
         <v>158</v>
@@ -3728,7 +3731,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="47" t="s">
         <v>157</v>
       </c>
@@ -3746,20 +3749,22 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="41">
         <v>45292</v>
       </c>
       <c r="B94" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C94" s="13"/>
+      <c r="C94" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D94" s="40"/>
       <c r="E94" s="9"/>
       <c r="F94" s="20"/>
-      <c r="G94" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G94" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H94" s="40">
         <v>1</v>
@@ -3770,7 +3775,7 @@
         <v>45293</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="41"/>
       <c r="B95" s="20" t="s">
         <v>57</v>
@@ -3789,11 +3794,13 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="41">
         <v>45323</v>
       </c>
-      <c r="B96" s="20"/>
+      <c r="B96" s="20" t="s">
+        <v>53</v>
+      </c>
       <c r="C96" s="13"/>
       <c r="D96" s="40"/>
       <c r="E96" s="9"/>
@@ -3805,9 +3812,11 @@
       <c r="H96" s="40"/>
       <c r="I96" s="9"/>
       <c r="J96" s="11"/>
-      <c r="K96" s="20"/>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K96" s="48">
+        <v>45330</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="41">
         <v>45352</v>
       </c>
@@ -3825,7 +3834,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="41">
         <v>45383</v>
       </c>
@@ -3843,7 +3852,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="41">
         <v>45413</v>
       </c>
@@ -3861,7 +3870,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="41">
         <v>45444</v>
       </c>
@@ -3879,7 +3888,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="41">
         <v>45474</v>
       </c>
@@ -3897,7 +3906,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="41"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -3913,7 +3922,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="41"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -3929,7 +3938,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="41"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -3945,7 +3954,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="41"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -3961,7 +3970,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="41"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -3977,7 +3986,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="41"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -3993,7 +4002,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="41"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4009,7 +4018,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="41"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -4025,7 +4034,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="41"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -4041,7 +4050,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="41"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -4057,7 +4066,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="41"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -4073,7 +4082,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="41"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -4089,7 +4098,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="41"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -4105,7 +4114,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="41"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -4121,7 +4130,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="41"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -4137,7 +4146,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="41"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -4153,7 +4162,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="41"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -4169,7 +4178,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="41"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -4185,7 +4194,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="41"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -4201,7 +4210,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="42"/>
       <c r="B121" s="15"/>
       <c r="C121" s="43"/>
@@ -4219,23 +4228,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4258,34 +4267,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K204"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3990" topLeftCell="A162" activePane="bottomLeft"/>
+      <pane ySplit="3984" topLeftCell="A162" activePane="bottomLeft"/>
       <selection activeCell="I9" sqref="I9"/>
       <selection pane="bottomLeft" activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -4297,16 +4306,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -4315,18 +4324,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="55">
         <v>43101</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -4337,16 +4346,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -4354,7 +4363,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -4367,24 +4376,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -4419,7 +4428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -4443,7 +4452,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="47" t="s">
         <v>43</v>
       </c>
@@ -4465,7 +4474,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="41">
         <v>43101</v>
       </c>
@@ -4487,7 +4496,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="41"/>
       <c r="B12" s="20" t="s">
         <v>57</v>
@@ -4509,7 +4518,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="41"/>
       <c r="B13" s="20" t="s">
         <v>66</v>
@@ -4529,7 +4538,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="41"/>
       <c r="B14" s="20" t="s">
         <v>55</v>
@@ -4551,7 +4560,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="41">
         <v>43132</v>
       </c>
@@ -4573,7 +4582,7 @@
         <v>43138</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="41"/>
       <c r="B16" s="20" t="s">
         <v>57</v>
@@ -4595,7 +4604,7 @@
         <v>43133</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="41"/>
       <c r="B17" s="20" t="s">
         <v>57</v>
@@ -4617,7 +4626,7 @@
         <v>43117</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="41"/>
       <c r="B18" s="20" t="s">
         <v>57</v>
@@ -4637,7 +4646,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="48"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="41"/>
       <c r="B19" s="20" t="s">
         <v>57</v>
@@ -4659,7 +4668,7 @@
         <v>43146</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="41"/>
       <c r="B20" s="20" t="s">
         <v>55</v>
@@ -4681,7 +4690,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="41"/>
       <c r="B21" s="20" t="s">
         <v>57</v>
@@ -4703,7 +4712,7 @@
         <v>43159</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="41">
         <v>43160</v>
       </c>
@@ -4725,7 +4734,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="41"/>
       <c r="B23" s="20" t="s">
         <v>71</v>
@@ -4747,7 +4756,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="41"/>
       <c r="B24" s="20" t="s">
         <v>55</v>
@@ -4769,7 +4778,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="41">
         <v>43191</v>
       </c>
@@ -4793,7 +4802,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="41"/>
       <c r="B26" s="20" t="s">
         <v>57</v>
@@ -4815,7 +4824,7 @@
         <v>43203</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="41"/>
       <c r="B27" s="20" t="s">
         <v>55</v>
@@ -4837,7 +4846,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="41"/>
       <c r="B28" s="20" t="s">
         <v>71</v>
@@ -4859,7 +4868,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="41"/>
       <c r="B29" s="20" t="s">
         <v>75</v>
@@ -4881,7 +4890,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="41"/>
       <c r="B30" s="20" t="s">
         <v>55</v>
@@ -4903,7 +4912,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="41">
         <v>43221</v>
       </c>
@@ -4927,7 +4936,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="41"/>
       <c r="B32" s="15" t="s">
         <v>71</v>
@@ -4949,7 +4958,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="41"/>
       <c r="B33" s="15" t="s">
         <v>71</v>
@@ -4971,7 +4980,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="41"/>
       <c r="B34" s="15" t="s">
         <v>84</v>
@@ -4991,7 +5000,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="15"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="41">
         <v>43252</v>
       </c>
@@ -5015,7 +5024,7 @@
         <v>43258</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="41"/>
       <c r="B36" s="15" t="s">
         <v>57</v>
@@ -5037,7 +5046,7 @@
         <v>43270</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="41"/>
       <c r="B37" s="15" t="s">
         <v>57</v>
@@ -5059,7 +5068,7 @@
         <v>43276</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="41"/>
       <c r="B38" s="15" t="s">
         <v>85</v>
@@ -5079,7 +5088,7 @@
       <c r="J38" s="12"/>
       <c r="K38" s="49"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="41">
         <v>43282</v>
       </c>
@@ -5103,7 +5112,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="41"/>
       <c r="B40" s="20" t="s">
         <v>57</v>
@@ -5123,7 +5132,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="41"/>
       <c r="B41" s="20" t="s">
         <v>87</v>
@@ -5143,7 +5152,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="41">
         <v>43313</v>
       </c>
@@ -5167,7 +5176,7 @@
         <v>43318</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="41"/>
       <c r="B43" s="20" t="s">
         <v>57</v>
@@ -5189,7 +5198,7 @@
         <v>43325</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="41"/>
       <c r="B44" s="20" t="s">
         <v>57</v>
@@ -5211,7 +5220,7 @@
         <v>43328</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="41"/>
       <c r="B45" s="20" t="s">
         <v>88</v>
@@ -5231,7 +5240,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="48"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="41">
         <v>43344</v>
       </c>
@@ -5255,7 +5264,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="41"/>
       <c r="B47" s="20" t="s">
         <v>55</v>
@@ -5277,7 +5286,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="41"/>
       <c r="B48" s="20" t="s">
         <v>90</v>
@@ -5295,7 +5304,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="48"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="41">
         <v>43374</v>
       </c>
@@ -5319,7 +5328,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="41"/>
       <c r="B50" s="20" t="s">
         <v>75</v>
@@ -5341,7 +5350,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="41"/>
       <c r="B51" s="20" t="s">
         <v>93</v>
@@ -5361,7 +5370,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="41">
         <v>43405</v>
       </c>
@@ -5385,7 +5394,7 @@
         <v>43425</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="41"/>
       <c r="B53" s="20" t="s">
         <v>55</v>
@@ -5407,7 +5416,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="41"/>
       <c r="B54" s="20" t="s">
         <v>95</v>
@@ -5425,7 +5434,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="48"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="41">
         <v>43435</v>
       </c>
@@ -5449,7 +5458,7 @@
         <v>43452</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="41"/>
       <c r="B56" s="20" t="s">
         <v>57</v>
@@ -5471,7 +5480,7 @@
         <v>43445</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="41"/>
       <c r="B57" s="20" t="s">
         <v>55</v>
@@ -5493,7 +5502,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="41"/>
       <c r="B58" s="20" t="s">
         <v>97</v>
@@ -5511,7 +5520,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="48"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="47" t="s">
         <v>44</v>
       </c>
@@ -5529,7 +5538,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="41">
         <v>43466</v>
       </c>
@@ -5551,7 +5560,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="41"/>
       <c r="B61" s="20" t="s">
         <v>71</v>
@@ -5573,7 +5582,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="41">
         <v>43497</v>
       </c>
@@ -5597,7 +5606,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="41"/>
       <c r="B63" s="20" t="s">
         <v>57</v>
@@ -5619,7 +5628,7 @@
         <v>43517</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="41"/>
       <c r="B64" s="20" t="s">
         <v>53</v>
@@ -5639,7 +5648,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="41"/>
       <c r="B65" s="20" t="s">
         <v>55</v>
@@ -5661,7 +5670,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="41">
         <v>43525</v>
       </c>
@@ -5685,7 +5694,7 @@
         <v>43531</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="41"/>
       <c r="B67" s="20" t="s">
         <v>71</v>
@@ -5707,7 +5716,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="41"/>
       <c r="B68" s="20" t="s">
         <v>57</v>
@@ -5729,7 +5738,7 @@
         <v>43552</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="41">
         <v>43556</v>
       </c>
@@ -5753,7 +5762,7 @@
         <v>43817</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="41"/>
       <c r="B70" s="20" t="s">
         <v>57</v>
@@ -5775,7 +5784,7 @@
         <v>43557</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="41"/>
       <c r="B71" s="20" t="s">
         <v>57</v>
@@ -5797,7 +5806,7 @@
         <v>43572</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="41"/>
       <c r="B72" s="20" t="s">
         <v>55</v>
@@ -5819,7 +5828,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="41">
         <v>43586</v>
       </c>
@@ -5843,7 +5852,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="41"/>
       <c r="B74" s="20" t="s">
         <v>75</v>
@@ -5865,7 +5874,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="41"/>
       <c r="B75" s="20" t="s">
         <v>57</v>
@@ -5887,7 +5896,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="41"/>
       <c r="B76" s="20" t="s">
         <v>57</v>
@@ -5909,7 +5918,7 @@
         <v>43601</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="41"/>
       <c r="B77" s="20" t="s">
         <v>55</v>
@@ -5931,7 +5940,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="41"/>
       <c r="B78" s="20" t="s">
         <v>57</v>
@@ -5953,7 +5962,7 @@
         <v>43615</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="41">
         <v>43617</v>
       </c>
@@ -5977,7 +5986,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="41"/>
       <c r="B80" s="20" t="s">
         <v>71</v>
@@ -5999,7 +6008,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="41"/>
       <c r="B81" s="20" t="s">
         <v>57</v>
@@ -6021,7 +6030,7 @@
         <v>43629</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="41"/>
       <c r="B82" s="20" t="s">
         <v>57</v>
@@ -6043,7 +6052,7 @@
         <v>43633</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="41"/>
       <c r="B83" s="20" t="s">
         <v>108</v>
@@ -6065,7 +6074,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="41"/>
       <c r="B84" s="20" t="s">
         <v>66</v>
@@ -6085,7 +6094,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="41">
         <v>43647</v>
       </c>
@@ -6109,7 +6118,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="41"/>
       <c r="B86" s="20" t="s">
         <v>57</v>
@@ -6131,7 +6140,7 @@
         <v>43663</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="41"/>
       <c r="B87" s="20" t="s">
         <v>57</v>
@@ -6153,7 +6162,7 @@
         <v>43668</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="41">
         <v>43678</v>
       </c>
@@ -6177,7 +6186,7 @@
         <v>43678</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="41"/>
       <c r="B89" s="20" t="s">
         <v>57</v>
@@ -6199,7 +6208,7 @@
         <v>43685</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="41"/>
       <c r="B90" s="20" t="s">
         <v>57</v>
@@ -6221,7 +6230,7 @@
         <v>43700</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="41"/>
       <c r="B91" s="20" t="s">
         <v>55</v>
@@ -6243,7 +6252,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="41">
         <v>43709</v>
       </c>
@@ -6267,7 +6276,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="41"/>
       <c r="B93" s="20" t="s">
         <v>55</v>
@@ -6289,7 +6298,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="41"/>
       <c r="B94" s="20" t="s">
         <v>55</v>
@@ -6311,7 +6320,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="41">
         <v>43739</v>
       </c>
@@ -6335,7 +6344,7 @@
         <v>43749</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="41"/>
       <c r="B96" s="20" t="s">
         <v>55</v>
@@ -6357,7 +6366,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="41"/>
       <c r="B97" s="20" t="s">
         <v>57</v>
@@ -6379,7 +6388,7 @@
         <v>43755</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="41"/>
       <c r="B98" s="20" t="s">
         <v>57</v>
@@ -6401,7 +6410,7 @@
         <v>43762</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="41"/>
       <c r="B99" s="20" t="s">
         <v>57</v>
@@ -6423,7 +6432,7 @@
         <v>43769</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="41">
         <v>43770</v>
       </c>
@@ -6447,7 +6456,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="41"/>
       <c r="B101" s="20" t="s">
         <v>57</v>
@@ -6469,7 +6478,7 @@
         <v>43777</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="41"/>
       <c r="B102" s="20" t="s">
         <v>57</v>
@@ -6491,7 +6500,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="41">
         <v>43800</v>
       </c>
@@ -6513,7 +6522,7 @@
         <v>43817</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="41"/>
       <c r="B104" s="20" t="s">
         <v>55</v>
@@ -6535,7 +6544,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="41"/>
       <c r="B105" s="20" t="s">
         <v>55</v>
@@ -6557,7 +6566,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="47" t="s">
         <v>45</v>
       </c>
@@ -6575,7 +6584,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="41">
         <v>43831</v>
       </c>
@@ -6597,7 +6606,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="41"/>
       <c r="B108" s="20" t="s">
         <v>71</v>
@@ -6619,7 +6628,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="41">
         <v>43891</v>
       </c>
@@ -6643,7 +6652,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="41"/>
       <c r="B110" s="20" t="s">
         <v>121</v>
@@ -6663,7 +6672,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="41"/>
       <c r="B111" s="20" t="s">
         <v>123</v>
@@ -6683,7 +6692,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="41">
         <v>43922</v>
       </c>
@@ -6707,7 +6716,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="41"/>
       <c r="B113" s="20" t="s">
         <v>47</v>
@@ -6729,7 +6738,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="41">
         <v>43952</v>
       </c>
@@ -6747,7 +6756,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="41">
         <v>43983</v>
       </c>
@@ -6765,7 +6774,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="41">
         <v>44013</v>
       </c>
@@ -6783,7 +6792,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="41">
         <v>44044</v>
       </c>
@@ -6807,7 +6816,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="41">
         <v>44075</v>
       </c>
@@ -6829,7 +6838,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="41">
         <v>44105</v>
       </c>
@@ -6847,7 +6856,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="41">
         <v>44136</v>
       </c>
@@ -6865,7 +6874,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="41">
         <v>44166</v>
       </c>
@@ -6889,7 +6898,7 @@
         <v>44173</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="41"/>
       <c r="B122" s="20" t="s">
         <v>55</v>
@@ -6911,7 +6920,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="41"/>
       <c r="B123" s="20" t="s">
         <v>71</v>
@@ -6933,7 +6942,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="47" t="s">
         <v>46</v>
       </c>
@@ -6951,7 +6960,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="41">
         <v>44197</v>
       </c>
@@ -6975,7 +6984,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="41">
         <v>44228</v>
       </c>
@@ -6997,7 +7006,7 @@
         <v>44249</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="41"/>
       <c r="B127" s="20" t="s">
         <v>53</v>
@@ -7017,7 +7026,7 @@
         <v>44215</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="41"/>
       <c r="B128" s="20" t="s">
         <v>55</v>
@@ -7039,7 +7048,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="41"/>
       <c r="B129" s="20" t="s">
         <v>71</v>
@@ -7061,7 +7070,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="41"/>
       <c r="B130" s="20" t="s">
         <v>57</v>
@@ -7083,7 +7092,7 @@
         <v>44229</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" s="41">
         <v>44378</v>
       </c>
@@ -7107,7 +7116,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" s="41"/>
       <c r="B132" s="20" t="s">
         <v>55</v>
@@ -7129,7 +7138,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133" s="41"/>
       <c r="B133" s="20" t="s">
         <v>55</v>
@@ -7151,7 +7160,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="41">
         <v>44440</v>
       </c>
@@ -7173,7 +7182,7 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="41">
         <v>44470</v>
       </c>
@@ -7197,7 +7206,7 @@
         <v>44489</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" s="41"/>
       <c r="B136" s="20" t="s">
         <v>136</v>
@@ -7219,7 +7228,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137" s="41"/>
       <c r="B137" s="20" t="s">
         <v>121</v>
@@ -7239,7 +7248,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" s="47" t="s">
         <v>52</v>
       </c>
@@ -7257,7 +7266,7 @@
       <c r="J138" s="11"/>
       <c r="K138" s="20"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" s="41">
         <v>44562</v>
       </c>
@@ -7281,7 +7290,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" s="41"/>
       <c r="B140" s="20" t="s">
         <v>57</v>
@@ -7303,7 +7312,7 @@
         <v>44589</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" s="41"/>
       <c r="B141" s="20" t="s">
         <v>55</v>
@@ -7325,7 +7334,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142" s="41">
         <v>44593</v>
       </c>
@@ -7349,7 +7358,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" s="41"/>
       <c r="B143" s="20" t="s">
         <v>55</v>
@@ -7371,7 +7380,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" s="41"/>
       <c r="B144" s="20" t="s">
         <v>71</v>
@@ -7393,7 +7402,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" s="41"/>
       <c r="B145" s="20" t="s">
         <v>55</v>
@@ -7415,7 +7424,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="41">
         <v>44652</v>
       </c>
@@ -7439,7 +7448,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" s="41"/>
       <c r="B147" s="20" t="s">
         <v>57</v>
@@ -7461,7 +7470,7 @@
         <v>44680</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" s="41">
         <v>44682</v>
       </c>
@@ -7485,7 +7494,7 @@
         <v>44704</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" s="41">
         <v>44713</v>
       </c>
@@ -7507,7 +7516,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150" s="41"/>
       <c r="B150" s="20" t="s">
         <v>55</v>
@@ -7529,7 +7538,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" s="41"/>
       <c r="B151" s="20" t="s">
         <v>57</v>
@@ -7551,7 +7560,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" s="41"/>
       <c r="B152" s="20" t="s">
         <v>57</v>
@@ -7573,7 +7582,7 @@
         <v>44764</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="41"/>
       <c r="B153" s="20" t="s">
         <v>55</v>
@@ -7595,7 +7604,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154" s="41"/>
       <c r="B154" s="20" t="s">
         <v>55</v>
@@ -7617,7 +7626,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" s="41">
         <v>44805</v>
       </c>
@@ -7641,7 +7650,7 @@
         <v>44811</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" s="41"/>
       <c r="B156" s="20" t="s">
         <v>57</v>
@@ -7663,7 +7672,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" s="41">
         <v>44835</v>
       </c>
@@ -7687,7 +7696,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" s="41"/>
       <c r="B158" s="20" t="s">
         <v>57</v>
@@ -7709,7 +7718,7 @@
         <v>44841</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" s="41"/>
       <c r="B159" s="20" t="s">
         <v>53</v>
@@ -7729,7 +7738,7 @@
         <v>44845</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" s="41"/>
       <c r="B160" s="20" t="s">
         <v>57</v>
@@ -7751,7 +7760,7 @@
         <v>44854</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" s="41"/>
       <c r="B161" s="20" t="s">
         <v>55</v>
@@ -7773,7 +7782,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" s="41">
         <v>44866</v>
       </c>
@@ -7795,7 +7804,7 @@
         <v>44893</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" s="41"/>
       <c r="B163" s="20" t="s">
         <v>57</v>
@@ -7817,7 +7826,7 @@
         <v>44876</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" s="41"/>
       <c r="B164" s="20" t="s">
         <v>57</v>
@@ -7839,7 +7848,7 @@
         <v>44887</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" s="41">
         <v>44896</v>
       </c>
@@ -7863,7 +7872,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" s="47" t="s">
         <v>145</v>
       </c>
@@ -7881,7 +7890,7 @@
       <c r="J166" s="11"/>
       <c r="K166" s="20"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" s="41">
         <v>44986</v>
       </c>
@@ -7905,7 +7914,7 @@
         <v>44995</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" s="41">
         <v>45017</v>
       </c>
@@ -7929,7 +7938,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" s="41">
         <v>45047</v>
       </c>
@@ -7947,7 +7956,7 @@
       <c r="J169" s="11"/>
       <c r="K169" s="20"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" s="41">
         <v>45078</v>
       </c>
@@ -7971,7 +7980,7 @@
         <v>45082</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171" s="41">
         <v>45139</v>
       </c>
@@ -7995,7 +8004,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" s="41"/>
       <c r="B172" s="20" t="s">
         <v>57</v>
@@ -8017,7 +8026,7 @@
         <v>45167</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" s="41">
         <v>45170</v>
       </c>
@@ -8041,7 +8050,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174" s="41">
         <v>45200</v>
       </c>
@@ -8065,7 +8074,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175" s="41"/>
       <c r="B175" s="20" t="s">
         <v>57</v>
@@ -8087,7 +8096,7 @@
         <v>45230</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176" s="41"/>
       <c r="B176" s="20"/>
       <c r="C176" s="13"/>
@@ -8103,7 +8112,7 @@
       <c r="J176" s="11"/>
       <c r="K176" s="20"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177" s="41"/>
       <c r="B177" s="20"/>
       <c r="C177" s="13"/>
@@ -8119,7 +8128,7 @@
       <c r="J177" s="11"/>
       <c r="K177" s="20"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178" s="41"/>
       <c r="B178" s="20"/>
       <c r="C178" s="13"/>
@@ -8135,7 +8144,7 @@
       <c r="J178" s="11"/>
       <c r="K178" s="20"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179" s="41"/>
       <c r="B179" s="20"/>
       <c r="C179" s="13"/>
@@ -8151,7 +8160,7 @@
       <c r="J179" s="11"/>
       <c r="K179" s="20"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180" s="41"/>
       <c r="B180" s="20"/>
       <c r="C180" s="13"/>
@@ -8167,7 +8176,7 @@
       <c r="J180" s="11"/>
       <c r="K180" s="20"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181" s="41"/>
       <c r="B181" s="20"/>
       <c r="C181" s="13"/>
@@ -8183,7 +8192,7 @@
       <c r="J181" s="11"/>
       <c r="K181" s="20"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182" s="41"/>
       <c r="B182" s="20"/>
       <c r="C182" s="13"/>
@@ -8199,7 +8208,7 @@
       <c r="J182" s="11"/>
       <c r="K182" s="20"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A183" s="41"/>
       <c r="B183" s="20"/>
       <c r="C183" s="13"/>
@@ -8215,7 +8224,7 @@
       <c r="J183" s="11"/>
       <c r="K183" s="20"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184" s="41"/>
       <c r="B184" s="20"/>
       <c r="C184" s="13"/>
@@ -8231,7 +8240,7 @@
       <c r="J184" s="11"/>
       <c r="K184" s="20"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185" s="41"/>
       <c r="B185" s="20"/>
       <c r="C185" s="13"/>
@@ -8247,7 +8256,7 @@
       <c r="J185" s="11"/>
       <c r="K185" s="20"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186" s="41"/>
       <c r="B186" s="20"/>
       <c r="C186" s="13"/>
@@ -8263,7 +8272,7 @@
       <c r="J186" s="11"/>
       <c r="K186" s="20"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187" s="41"/>
       <c r="B187" s="20"/>
       <c r="C187" s="13"/>
@@ -8279,7 +8288,7 @@
       <c r="J187" s="11"/>
       <c r="K187" s="20"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188" s="41"/>
       <c r="B188" s="20"/>
       <c r="C188" s="13"/>
@@ -8295,7 +8304,7 @@
       <c r="J188" s="11"/>
       <c r="K188" s="20"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189" s="41"/>
       <c r="B189" s="20"/>
       <c r="C189" s="13"/>
@@ -8311,7 +8320,7 @@
       <c r="J189" s="11"/>
       <c r="K189" s="20"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A190" s="41"/>
       <c r="B190" s="20"/>
       <c r="C190" s="13"/>
@@ -8327,7 +8336,7 @@
       <c r="J190" s="11"/>
       <c r="K190" s="20"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A191" s="41"/>
       <c r="B191" s="20"/>
       <c r="C191" s="13"/>
@@ -8343,7 +8352,7 @@
       <c r="J191" s="11"/>
       <c r="K191" s="20"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A192" s="41"/>
       <c r="B192" s="20"/>
       <c r="C192" s="13"/>
@@ -8359,7 +8368,7 @@
       <c r="J192" s="11"/>
       <c r="K192" s="20"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A193" s="41"/>
       <c r="B193" s="20"/>
       <c r="C193" s="13"/>
@@ -8375,7 +8384,7 @@
       <c r="J193" s="11"/>
       <c r="K193" s="20"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A194" s="41"/>
       <c r="B194" s="20"/>
       <c r="C194" s="13"/>
@@ -8391,7 +8400,7 @@
       <c r="J194" s="11"/>
       <c r="K194" s="20"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A195" s="41"/>
       <c r="B195" s="20"/>
       <c r="C195" s="13"/>
@@ -8407,7 +8416,7 @@
       <c r="J195" s="11"/>
       <c r="K195" s="20"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A196" s="41"/>
       <c r="B196" s="20"/>
       <c r="C196" s="13"/>
@@ -8423,7 +8432,7 @@
       <c r="J196" s="11"/>
       <c r="K196" s="20"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A197" s="41"/>
       <c r="B197" s="20"/>
       <c r="C197" s="13"/>
@@ -8439,7 +8448,7 @@
       <c r="J197" s="11"/>
       <c r="K197" s="20"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A198" s="41"/>
       <c r="B198" s="20"/>
       <c r="C198" s="13"/>
@@ -8455,7 +8464,7 @@
       <c r="J198" s="11"/>
       <c r="K198" s="20"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A199" s="41"/>
       <c r="B199" s="20"/>
       <c r="C199" s="13"/>
@@ -8471,7 +8480,7 @@
       <c r="J199" s="11"/>
       <c r="K199" s="20"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A200" s="41"/>
       <c r="B200" s="20"/>
       <c r="C200" s="13"/>
@@ -8487,7 +8496,7 @@
       <c r="J200" s="11"/>
       <c r="K200" s="20"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A201" s="41"/>
       <c r="B201" s="20"/>
       <c r="C201" s="13"/>
@@ -8503,7 +8512,7 @@
       <c r="J201" s="11"/>
       <c r="K201" s="20"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A202" s="41"/>
       <c r="B202" s="20"/>
       <c r="C202" s="13"/>
@@ -8519,7 +8528,7 @@
       <c r="J202" s="11"/>
       <c r="K202" s="20"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A203" s="41"/>
       <c r="B203" s="20"/>
       <c r="C203" s="13"/>
@@ -8535,7 +8544,7 @@
       <c r="J203" s="11"/>
       <c r="K203" s="20"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A204" s="42"/>
       <c r="B204" s="15"/>
       <c r="C204" s="43"/>
@@ -8566,10 +8575,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8592,28 +8601,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="38" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="38" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -8626,7 +8635,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -8655,7 +8664,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>53.343000000000004</v>
       </c>
@@ -8687,7 +8696,7 @@
         <v>0.20799999999999974</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E4" s="1">
         <f>IF(E3=0,0,IF(ISBLANK(E3),"",VLOOKUP(E3,E7:F14,2)))</f>
         <v>0</v>
@@ -8702,10 +8711,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C6" s="39" t="s">
         <v>28</v>
       </c>
@@ -8725,7 +8734,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" s="38">
         <v>1</v>
       </c>
@@ -8751,7 +8760,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="38">
         <v>2</v>
       </c>
@@ -8777,7 +8786,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="38">
         <v>3</v>
       </c>
@@ -8803,7 +8812,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="38">
         <v>4</v>
       </c>
@@ -8829,7 +8838,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="38">
         <v>5</v>
       </c>
@@ -8855,7 +8864,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="38">
         <v>6</v>
       </c>
@@ -8881,7 +8890,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="38">
         <v>7</v>
       </c>
@@ -8907,7 +8916,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="38">
         <v>8</v>
       </c>
@@ -8933,7 +8942,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="38">
         <v>9</v>
       </c>
@@ -8953,7 +8962,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" s="38">
         <v>10</v>
       </c>
@@ -8973,7 +8982,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="38">
         <v>11</v>
       </c>
@@ -8993,7 +9002,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="38">
         <v>12</v>
       </c>
@@ -9014,7 +9023,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="38">
         <v>13</v>
       </c>
@@ -9035,7 +9044,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="38">
         <v>14</v>
       </c>
@@ -9056,7 +9065,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="38">
         <v>15</v>
       </c>
@@ -9077,7 +9086,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="38">
         <v>16</v>
       </c>
@@ -9098,7 +9107,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="38">
         <v>17</v>
       </c>
@@ -9119,7 +9128,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="38">
         <v>18</v>
       </c>
@@ -9140,7 +9149,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="38">
         <v>19</v>
       </c>
@@ -9161,7 +9170,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="38">
         <v>20</v>
       </c>
@@ -9182,7 +9191,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="38">
         <v>21</v>
       </c>
@@ -9203,7 +9212,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="38">
         <v>22</v>
       </c>
@@ -9224,7 +9233,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="38">
         <v>23</v>
       </c>
@@ -9245,7 +9254,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="38">
         <v>24</v>
       </c>
@@ -9266,7 +9275,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="38">
         <v>25</v>
       </c>
@@ -9287,7 +9296,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="38">
         <v>26</v>
       </c>
@@ -9308,7 +9317,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="38">
         <v>27</v>
       </c>
@@ -9329,7 +9338,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C34" s="38">
         <v>28</v>
       </c>
@@ -9350,7 +9359,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C35" s="38">
         <v>29</v>
       </c>
@@ -9371,7 +9380,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="38">
         <v>30</v>
       </c>
@@ -9392,7 +9401,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="38">
         <v>31</v>
       </c>
@@ -9413,7 +9422,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="38">
         <v>32</v>
       </c>
@@ -9422,7 +9431,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="38">
         <v>33</v>
       </c>
@@ -9431,7 +9440,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="38">
         <v>34</v>
       </c>
@@ -9440,7 +9449,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="38">
         <v>35</v>
       </c>
@@ -9449,7 +9458,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="38">
         <v>36</v>
       </c>
@@ -9458,7 +9467,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="38">
         <v>37</v>
       </c>
@@ -9467,7 +9476,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="38">
         <v>38</v>
       </c>
@@ -9476,7 +9485,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C45" s="38">
         <v>39</v>
       </c>
@@ -9485,7 +9494,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="38">
         <v>40</v>
       </c>
@@ -9494,7 +9503,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="38">
         <v>41</v>
       </c>
@@ -9503,7 +9512,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="38">
         <v>42</v>
       </c>
@@ -9512,7 +9521,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="38">
         <v>43</v>
       </c>
@@ -9521,7 +9530,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="38">
         <v>44</v>
       </c>
@@ -9530,7 +9539,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="38">
         <v>45</v>
       </c>
@@ -9539,7 +9548,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="38">
         <v>46</v>
       </c>
@@ -9548,7 +9557,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C53" s="38">
         <v>47</v>
       </c>
@@ -9557,7 +9566,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="38">
         <v>48</v>
       </c>
@@ -9566,7 +9575,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C55" s="38">
         <v>49</v>
       </c>
@@ -9575,7 +9584,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="38">
         <v>50</v>
       </c>
@@ -9584,7 +9593,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="38">
         <v>51</v>
       </c>
@@ -9593,7 +9602,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="38">
         <v>52</v>
       </c>
@@ -9602,7 +9611,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C59" s="38">
         <v>53</v>
       </c>
@@ -9611,7 +9620,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C60" s="38">
         <v>54</v>
       </c>
@@ -9620,7 +9629,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C61" s="38">
         <v>55</v>
       </c>
@@ -9629,7 +9638,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C62" s="38">
         <v>56</v>
       </c>
@@ -9638,7 +9647,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C63" s="38">
         <v>57</v>
       </c>
@@ -9647,7 +9656,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C64" s="38">
         <v>58</v>
       </c>
@@ -9656,7 +9665,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C65" s="38">
         <v>59</v>
       </c>
@@ -9665,7 +9674,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C66" s="38">
         <v>60</v>
       </c>
@@ -9674,7 +9683,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>

<commit_message>
update leave card 02/14/2024 4:35pm
</commit_message>
<xml_diff>
--- a/CASUAL/LA ACCOUNTING/ABELA, IMELDA.xlsx
+++ b/CASUAL/LA ACCOUNTING/ABELA, IMELDA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA ACCOUNTING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA ACCOUNTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B87C427-E5A3-4CA5-8E6F-6DF09D147856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="2018 LEAVE CREDITS" sheetId="4" r:id="rId1"/>
@@ -27,7 +26,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="161">
   <si>
     <t>PERIOD</t>
   </si>
@@ -525,7 +524,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -903,17 +902,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -923,6 +919,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1434,7 +1433,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1451,25 +1450,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K121" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K122" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
+    <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1481,25 +1480,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K204" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K204" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1806,34 +1805,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K121"/>
+  <dimension ref="A2:K122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3696" topLeftCell="A88" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A88" activePane="bottomLeft"/>
       <selection activeCell="I9" sqref="I9"/>
       <selection pane="bottomLeft" activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -1845,16 +1844,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -1863,18 +1862,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>43101</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -1885,16 +1884,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -1902,7 +1901,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -1915,24 +1914,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -1967,7 +1966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -1986,12 +1985,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
-        <v>89.25</v>
+        <v>88.25</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>43</v>
       </c>
@@ -2013,7 +2012,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="41">
         <v>43101</v>
       </c>
@@ -2033,7 +2032,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>43132</v>
       </c>
@@ -2059,7 +2058,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="41">
         <v>43160</v>
       </c>
@@ -2079,7 +2078,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="41">
         <v>43191</v>
       </c>
@@ -2099,7 +2098,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="41">
         <v>43221</v>
       </c>
@@ -2119,7 +2118,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="41">
         <v>43252</v>
       </c>
@@ -2139,7 +2138,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="41">
         <v>43282</v>
       </c>
@@ -2159,7 +2158,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="41">
         <v>43313</v>
       </c>
@@ -2179,7 +2178,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="41">
         <v>43344</v>
       </c>
@@ -2199,7 +2198,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="41">
         <v>43374</v>
       </c>
@@ -2219,7 +2218,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="41">
         <v>43405</v>
       </c>
@@ -2239,7 +2238,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="41">
         <v>43435</v>
       </c>
@@ -2259,7 +2258,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
         <v>44</v>
       </c>
@@ -2277,7 +2276,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="41">
         <v>43466</v>
       </c>
@@ -2303,7 +2302,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="41">
         <v>43497</v>
       </c>
@@ -2323,7 +2322,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="41">
         <v>43525</v>
       </c>
@@ -2343,7 +2342,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="41">
         <v>43556</v>
       </c>
@@ -2363,7 +2362,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="41">
         <v>43586</v>
       </c>
@@ -2383,7 +2382,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="41">
         <v>43617</v>
       </c>
@@ -2403,7 +2402,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="41">
         <v>43647</v>
       </c>
@@ -2423,7 +2422,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="41">
         <v>43678</v>
       </c>
@@ -2443,7 +2442,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="41">
         <v>43709</v>
       </c>
@@ -2463,7 +2462,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="41">
         <v>43739</v>
       </c>
@@ -2483,7 +2482,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="41">
         <v>43770</v>
       </c>
@@ -2503,7 +2502,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="41">
         <v>43800</v>
       </c>
@@ -2523,7 +2522,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="47" t="s">
         <v>45</v>
       </c>
@@ -2541,7 +2540,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="41">
         <v>43831</v>
       </c>
@@ -2565,7 +2564,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="41">
         <v>43862</v>
       </c>
@@ -2585,7 +2584,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="41">
         <v>43891</v>
       </c>
@@ -2605,7 +2604,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="41">
         <v>43922</v>
       </c>
@@ -2625,7 +2624,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="41">
         <v>43952</v>
       </c>
@@ -2645,7 +2644,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="41">
         <v>43983</v>
       </c>
@@ -2665,7 +2664,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="41">
         <v>44013</v>
       </c>
@@ -2685,7 +2684,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="41">
         <v>44044</v>
       </c>
@@ -2705,7 +2704,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="41">
         <v>44075</v>
       </c>
@@ -2725,7 +2724,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="41">
         <v>44105</v>
       </c>
@@ -2745,7 +2744,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="41">
         <v>44136</v>
       </c>
@@ -2765,7 +2764,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="41">
         <v>44166</v>
       </c>
@@ -2785,7 +2784,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="47" t="s">
         <v>46</v>
       </c>
@@ -2803,7 +2802,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="41">
         <v>44197</v>
       </c>
@@ -2823,7 +2822,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="41">
         <v>44228</v>
       </c>
@@ -2847,7 +2846,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="41"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13">
@@ -2865,7 +2864,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="41">
         <v>44256</v>
       </c>
@@ -2885,7 +2884,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="41">
         <v>44287</v>
       </c>
@@ -2905,7 +2904,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="41">
         <v>44317</v>
       </c>
@@ -2925,7 +2924,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="41">
         <v>44348</v>
       </c>
@@ -2945,7 +2944,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="41">
         <v>44378</v>
       </c>
@@ -2965,7 +2964,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="41">
         <v>44409</v>
       </c>
@@ -2985,7 +2984,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="41">
         <v>44440</v>
       </c>
@@ -3005,7 +3004,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="41">
         <v>44470</v>
       </c>
@@ -3031,7 +3030,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="41">
         <v>44501</v>
       </c>
@@ -3051,7 +3050,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="41">
         <v>44531</v>
       </c>
@@ -3071,7 +3070,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="47" t="s">
         <v>52</v>
       </c>
@@ -3089,7 +3088,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="41">
         <v>44562</v>
       </c>
@@ -3109,7 +3108,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="41">
         <v>44593</v>
       </c>
@@ -3129,7 +3128,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="41">
         <v>44621</v>
       </c>
@@ -3153,7 +3152,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="41">
         <v>44652</v>
       </c>
@@ -3173,7 +3172,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="41"/>
       <c r="B68" s="20" t="s">
         <v>155</v>
@@ -3193,7 +3192,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="41">
         <v>44682</v>
       </c>
@@ -3217,7 +3216,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="41">
         <v>44713</v>
       </c>
@@ -3241,7 +3240,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="41">
         <v>44743</v>
       </c>
@@ -3265,7 +3264,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="41">
         <v>44774</v>
       </c>
@@ -3289,7 +3288,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="41">
         <v>44805</v>
       </c>
@@ -3313,7 +3312,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="41">
         <v>44835</v>
       </c>
@@ -3339,7 +3338,7 @@
         <v>44855</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="41"/>
       <c r="B75" s="20" t="s">
         <v>149</v>
@@ -3359,7 +3358,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="48"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="41">
         <v>44866</v>
       </c>
@@ -3385,7 +3384,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="41"/>
       <c r="B77" s="20" t="s">
         <v>62</v>
@@ -3407,7 +3406,7 @@
         <v>44894</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="41">
         <v>44896</v>
       </c>
@@ -3431,7 +3430,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="47" t="s">
         <v>145</v>
       </c>
@@ -3449,7 +3448,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="41">
         <v>44927</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="41">
         <v>44958</v>
       </c>
@@ -3495,7 +3494,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="41">
         <v>44986</v>
       </c>
@@ -3515,7 +3514,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="41">
         <v>45017</v>
       </c>
@@ -3535,7 +3534,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="41">
         <v>45047</v>
       </c>
@@ -3555,7 +3554,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="41">
         <v>45078</v>
       </c>
@@ -3575,7 +3574,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="41">
         <v>45108</v>
       </c>
@@ -3595,7 +3594,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="41">
         <v>45139</v>
       </c>
@@ -3615,7 +3614,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="48"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="41">
         <v>45170</v>
       </c>
@@ -3635,7 +3634,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="41">
         <v>45200</v>
       </c>
@@ -3661,7 +3660,7 @@
         <v>45233</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="41">
         <v>45231</v>
       </c>
@@ -3685,7 +3684,7 @@
         <v>45254</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="41">
         <v>45261</v>
       </c>
@@ -3709,7 +3708,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="41"/>
       <c r="B92" s="20" t="s">
         <v>158</v>
@@ -3731,7 +3730,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="47" t="s">
         <v>157</v>
       </c>
@@ -3749,7 +3748,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="41">
         <v>45292</v>
       </c>
@@ -3775,7 +3774,7 @@
         <v>45293</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="41"/>
       <c r="B95" s="20" t="s">
         <v>57</v>
@@ -3794,7 +3793,7 @@
         <v>45301</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="41">
         <v>45323</v>
       </c>
@@ -3816,11 +3815,11 @@
         <v>45330</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A97" s="41">
-        <v>45352</v>
-      </c>
-      <c r="B97" s="20"/>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="41"/>
+      <c r="B97" s="20" t="s">
+        <v>57</v>
+      </c>
       <c r="C97" s="13"/>
       <c r="D97" s="40"/>
       <c r="E97" s="9"/>
@@ -3829,14 +3828,18 @@
         <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H97" s="40"/>
+      <c r="H97" s="40">
+        <v>1</v>
+      </c>
       <c r="I97" s="9"/>
       <c r="J97" s="11"/>
-      <c r="K97" s="20"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K97" s="48">
+        <v>45334</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="41">
-        <v>45383</v>
+        <v>45352</v>
       </c>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -3852,9 +3855,9 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="41">
-        <v>45413</v>
+        <v>45383</v>
       </c>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -3870,9 +3873,9 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="41">
-        <v>45444</v>
+        <v>45413</v>
       </c>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -3888,9 +3891,9 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="41">
-        <v>45474</v>
+        <v>45444</v>
       </c>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -3906,8 +3909,10 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A102" s="41"/>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="41">
+        <v>45474</v>
+      </c>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
       <c r="D102" s="40"/>
@@ -3922,7 +3927,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="41"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -3938,7 +3943,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="41"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -3954,7 +3959,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="41"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -3970,7 +3975,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="41"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -3986,7 +3991,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="41"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -4002,7 +4007,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="41"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4018,7 +4023,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="41"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -4034,7 +4039,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="41"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -4050,7 +4055,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="41"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -4066,7 +4071,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="41"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -4082,7 +4087,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="41"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -4098,7 +4103,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="41"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -4114,7 +4119,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="41"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -4130,7 +4135,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="41"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -4146,7 +4151,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="41"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -4162,7 +4167,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="41"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -4178,7 +4183,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="41"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -4194,7 +4199,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="41"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -4210,41 +4215,57 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A121" s="42"/>
-      <c r="B121" s="15"/>
-      <c r="C121" s="43"/>
-      <c r="D121" s="44"/>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" s="41"/>
+      <c r="B121" s="20"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="40"/>
       <c r="E121" s="9"/>
-      <c r="F121" s="15"/>
-      <c r="G121" s="43" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H121" s="44"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H121" s="40"/>
       <c r="I121" s="9"/>
-      <c r="J121" s="12"/>
-      <c r="K121" s="15"/>
+      <c r="J121" s="11"/>
+      <c r="K121" s="20"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" s="42"/>
+      <c r="B122" s="15"/>
+      <c r="C122" s="43"/>
+      <c r="D122" s="44"/>
+      <c r="E122" s="9"/>
+      <c r="F122" s="15"/>
+      <c r="G122" s="43" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H122" s="44"/>
+      <c r="I122" s="9"/>
+      <c r="J122" s="12"/>
+      <c r="K122" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4267,34 +4288,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K204"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3984" topLeftCell="A162" activePane="bottomLeft"/>
+      <pane ySplit="3990" topLeftCell="A162" activePane="bottomLeft"/>
       <selection activeCell="I9" sqref="I9"/>
       <selection pane="bottomLeft" activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -4306,16 +4327,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -4324,18 +4345,18 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>43101</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -4346,16 +4367,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -4363,7 +4384,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -4376,24 +4397,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -4428,7 +4449,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -4452,7 +4473,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>43</v>
       </c>
@@ -4474,7 +4495,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="41">
         <v>43101</v>
       </c>
@@ -4496,7 +4517,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="41"/>
       <c r="B12" s="20" t="s">
         <v>57</v>
@@ -4518,7 +4539,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="41"/>
       <c r="B13" s="20" t="s">
         <v>66</v>
@@ -4538,7 +4559,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
       <c r="B14" s="20" t="s">
         <v>55</v>
@@ -4560,7 +4581,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="41">
         <v>43132</v>
       </c>
@@ -4582,7 +4603,7 @@
         <v>43138</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="41"/>
       <c r="B16" s="20" t="s">
         <v>57</v>
@@ -4604,7 +4625,7 @@
         <v>43133</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
       <c r="B17" s="20" t="s">
         <v>57</v>
@@ -4626,7 +4647,7 @@
         <v>43117</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>
       <c r="B18" s="20" t="s">
         <v>57</v>
@@ -4646,7 +4667,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="48"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
       <c r="B19" s="20" t="s">
         <v>57</v>
@@ -4668,7 +4689,7 @@
         <v>43146</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="41"/>
       <c r="B20" s="20" t="s">
         <v>55</v>
@@ -4690,7 +4711,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="41"/>
       <c r="B21" s="20" t="s">
         <v>57</v>
@@ -4712,7 +4733,7 @@
         <v>43159</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="41">
         <v>43160</v>
       </c>
@@ -4734,7 +4755,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
       <c r="B23" s="20" t="s">
         <v>71</v>
@@ -4756,7 +4777,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="41"/>
       <c r="B24" s="20" t="s">
         <v>55</v>
@@ -4778,7 +4799,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="41">
         <v>43191</v>
       </c>
@@ -4802,7 +4823,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="41"/>
       <c r="B26" s="20" t="s">
         <v>57</v>
@@ -4824,7 +4845,7 @@
         <v>43203</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
       <c r="B27" s="20" t="s">
         <v>55</v>
@@ -4846,7 +4867,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="41"/>
       <c r="B28" s="20" t="s">
         <v>71</v>
@@ -4868,7 +4889,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="41"/>
       <c r="B29" s="20" t="s">
         <v>75</v>
@@ -4890,7 +4911,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="41"/>
       <c r="B30" s="20" t="s">
         <v>55</v>
@@ -4912,7 +4933,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="41">
         <v>43221</v>
       </c>
@@ -4936,7 +4957,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="41"/>
       <c r="B32" s="15" t="s">
         <v>71</v>
@@ -4958,7 +4979,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="41"/>
       <c r="B33" s="15" t="s">
         <v>71</v>
@@ -4980,7 +5001,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="41"/>
       <c r="B34" s="15" t="s">
         <v>84</v>
@@ -5000,7 +5021,7 @@
       <c r="J34" s="12"/>
       <c r="K34" s="15"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="41">
         <v>43252</v>
       </c>
@@ -5024,7 +5045,7 @@
         <v>43258</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="41"/>
       <c r="B36" s="15" t="s">
         <v>57</v>
@@ -5046,7 +5067,7 @@
         <v>43270</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="41"/>
       <c r="B37" s="15" t="s">
         <v>57</v>
@@ -5068,7 +5089,7 @@
         <v>43276</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="41"/>
       <c r="B38" s="15" t="s">
         <v>85</v>
@@ -5088,7 +5109,7 @@
       <c r="J38" s="12"/>
       <c r="K38" s="49"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="41">
         <v>43282</v>
       </c>
@@ -5112,7 +5133,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="41"/>
       <c r="B40" s="20" t="s">
         <v>57</v>
@@ -5132,7 +5153,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="41"/>
       <c r="B41" s="20" t="s">
         <v>87</v>
@@ -5152,7 +5173,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="41">
         <v>43313</v>
       </c>
@@ -5176,7 +5197,7 @@
         <v>43318</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="41"/>
       <c r="B43" s="20" t="s">
         <v>57</v>
@@ -5198,7 +5219,7 @@
         <v>43325</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="41"/>
       <c r="B44" s="20" t="s">
         <v>57</v>
@@ -5220,7 +5241,7 @@
         <v>43328</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="41"/>
       <c r="B45" s="20" t="s">
         <v>88</v>
@@ -5240,7 +5261,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="48"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="41">
         <v>43344</v>
       </c>
@@ -5264,7 +5285,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="41"/>
       <c r="B47" s="20" t="s">
         <v>55</v>
@@ -5286,7 +5307,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="41"/>
       <c r="B48" s="20" t="s">
         <v>90</v>
@@ -5304,7 +5325,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="48"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="41">
         <v>43374</v>
       </c>
@@ -5328,7 +5349,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="41"/>
       <c r="B50" s="20" t="s">
         <v>75</v>
@@ -5350,7 +5371,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="41"/>
       <c r="B51" s="20" t="s">
         <v>93</v>
@@ -5370,7 +5391,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="41">
         <v>43405</v>
       </c>
@@ -5394,7 +5415,7 @@
         <v>43425</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="41"/>
       <c r="B53" s="20" t="s">
         <v>55</v>
@@ -5416,7 +5437,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="41"/>
       <c r="B54" s="20" t="s">
         <v>95</v>
@@ -5434,7 +5455,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="48"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="41">
         <v>43435</v>
       </c>
@@ -5458,7 +5479,7 @@
         <v>43452</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="41"/>
       <c r="B56" s="20" t="s">
         <v>57</v>
@@ -5480,7 +5501,7 @@
         <v>43445</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="41"/>
       <c r="B57" s="20" t="s">
         <v>55</v>
@@ -5502,7 +5523,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="41"/>
       <c r="B58" s="20" t="s">
         <v>97</v>
@@ -5520,7 +5541,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="48"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="47" t="s">
         <v>44</v>
       </c>
@@ -5538,7 +5559,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="41">
         <v>43466</v>
       </c>
@@ -5560,7 +5581,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="41"/>
       <c r="B61" s="20" t="s">
         <v>71</v>
@@ -5582,7 +5603,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="41">
         <v>43497</v>
       </c>
@@ -5606,7 +5627,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="41"/>
       <c r="B63" s="20" t="s">
         <v>57</v>
@@ -5628,7 +5649,7 @@
         <v>43517</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="41"/>
       <c r="B64" s="20" t="s">
         <v>53</v>
@@ -5648,7 +5669,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="41"/>
       <c r="B65" s="20" t="s">
         <v>55</v>
@@ -5670,7 +5691,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="41">
         <v>43525</v>
       </c>
@@ -5694,7 +5715,7 @@
         <v>43531</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="41"/>
       <c r="B67" s="20" t="s">
         <v>71</v>
@@ -5716,7 +5737,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="41"/>
       <c r="B68" s="20" t="s">
         <v>57</v>
@@ -5738,7 +5759,7 @@
         <v>43552</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="41">
         <v>43556</v>
       </c>
@@ -5762,7 +5783,7 @@
         <v>43817</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="41"/>
       <c r="B70" s="20" t="s">
         <v>57</v>
@@ -5784,7 +5805,7 @@
         <v>43557</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="41"/>
       <c r="B71" s="20" t="s">
         <v>57</v>
@@ -5806,7 +5827,7 @@
         <v>43572</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="41"/>
       <c r="B72" s="20" t="s">
         <v>55</v>
@@ -5828,7 +5849,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="41">
         <v>43586</v>
       </c>
@@ -5852,7 +5873,7 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="41"/>
       <c r="B74" s="20" t="s">
         <v>75</v>
@@ -5874,7 +5895,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="41"/>
       <c r="B75" s="20" t="s">
         <v>57</v>
@@ -5896,7 +5917,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="41"/>
       <c r="B76" s="20" t="s">
         <v>57</v>
@@ -5918,7 +5939,7 @@
         <v>43601</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="41"/>
       <c r="B77" s="20" t="s">
         <v>55</v>
@@ -5940,7 +5961,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="41"/>
       <c r="B78" s="20" t="s">
         <v>57</v>
@@ -5962,7 +5983,7 @@
         <v>43615</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="41">
         <v>43617</v>
       </c>
@@ -5986,7 +6007,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="41"/>
       <c r="B80" s="20" t="s">
         <v>71</v>
@@ -6008,7 +6029,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="41"/>
       <c r="B81" s="20" t="s">
         <v>57</v>
@@ -6030,7 +6051,7 @@
         <v>43629</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="41"/>
       <c r="B82" s="20" t="s">
         <v>57</v>
@@ -6052,7 +6073,7 @@
         <v>43633</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="41"/>
       <c r="B83" s="20" t="s">
         <v>108</v>
@@ -6074,7 +6095,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="41"/>
       <c r="B84" s="20" t="s">
         <v>66</v>
@@ -6094,7 +6115,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="41">
         <v>43647</v>
       </c>
@@ -6118,7 +6139,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="41"/>
       <c r="B86" s="20" t="s">
         <v>57</v>
@@ -6140,7 +6161,7 @@
         <v>43663</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="41"/>
       <c r="B87" s="20" t="s">
         <v>57</v>
@@ -6162,7 +6183,7 @@
         <v>43668</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="41">
         <v>43678</v>
       </c>
@@ -6186,7 +6207,7 @@
         <v>43678</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="41"/>
       <c r="B89" s="20" t="s">
         <v>57</v>
@@ -6208,7 +6229,7 @@
         <v>43685</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="41"/>
       <c r="B90" s="20" t="s">
         <v>57</v>
@@ -6230,7 +6251,7 @@
         <v>43700</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="41"/>
       <c r="B91" s="20" t="s">
         <v>55</v>
@@ -6252,7 +6273,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="41">
         <v>43709</v>
       </c>
@@ -6276,7 +6297,7 @@
         <v>43725</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="41"/>
       <c r="B93" s="20" t="s">
         <v>55</v>
@@ -6298,7 +6319,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="41"/>
       <c r="B94" s="20" t="s">
         <v>55</v>
@@ -6320,7 +6341,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="41">
         <v>43739</v>
       </c>
@@ -6344,7 +6365,7 @@
         <v>43749</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="41"/>
       <c r="B96" s="20" t="s">
         <v>55</v>
@@ -6366,7 +6387,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="41"/>
       <c r="B97" s="20" t="s">
         <v>57</v>
@@ -6388,7 +6409,7 @@
         <v>43755</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="41"/>
       <c r="B98" s="20" t="s">
         <v>57</v>
@@ -6410,7 +6431,7 @@
         <v>43762</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="41"/>
       <c r="B99" s="20" t="s">
         <v>57</v>
@@ -6432,7 +6453,7 @@
         <v>43769</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="41">
         <v>43770</v>
       </c>
@@ -6456,7 +6477,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="41"/>
       <c r="B101" s="20" t="s">
         <v>57</v>
@@ -6478,7 +6499,7 @@
         <v>43777</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="41"/>
       <c r="B102" s="20" t="s">
         <v>57</v>
@@ -6500,7 +6521,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="41">
         <v>43800</v>
       </c>
@@ -6522,7 +6543,7 @@
         <v>43817</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="41"/>
       <c r="B104" s="20" t="s">
         <v>55</v>
@@ -6544,7 +6565,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="41"/>
       <c r="B105" s="20" t="s">
         <v>55</v>
@@ -6566,7 +6587,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="47" t="s">
         <v>45</v>
       </c>
@@ -6584,7 +6605,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="41">
         <v>43831</v>
       </c>
@@ -6606,7 +6627,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="41"/>
       <c r="B108" s="20" t="s">
         <v>71</v>
@@ -6628,7 +6649,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="41">
         <v>43891</v>
       </c>
@@ -6652,7 +6673,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="41"/>
       <c r="B110" s="20" t="s">
         <v>121</v>
@@ -6672,7 +6693,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="41"/>
       <c r="B111" s="20" t="s">
         <v>123</v>
@@ -6692,7 +6713,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="41">
         <v>43922</v>
       </c>
@@ -6716,7 +6737,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="41"/>
       <c r="B113" s="20" t="s">
         <v>47</v>
@@ -6738,7 +6759,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="41">
         <v>43952</v>
       </c>
@@ -6756,7 +6777,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="41">
         <v>43983</v>
       </c>
@@ -6774,7 +6795,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="41">
         <v>44013</v>
       </c>
@@ -6792,7 +6813,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="41">
         <v>44044</v>
       </c>
@@ -6816,7 +6837,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="41">
         <v>44075</v>
       </c>
@@ -6838,7 +6859,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="41">
         <v>44105</v>
       </c>
@@ -6856,7 +6877,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="41">
         <v>44136</v>
       </c>
@@ -6874,7 +6895,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="41">
         <v>44166</v>
       </c>
@@ -6898,7 +6919,7 @@
         <v>44173</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="41"/>
       <c r="B122" s="20" t="s">
         <v>55</v>
@@ -6920,7 +6941,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="41"/>
       <c r="B123" s="20" t="s">
         <v>71</v>
@@ -6942,7 +6963,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="47" t="s">
         <v>46</v>
       </c>
@@ -6960,7 +6981,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="41">
         <v>44197</v>
       </c>
@@ -6984,7 +7005,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="41">
         <v>44228</v>
       </c>
@@ -7006,7 +7027,7 @@
         <v>44249</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="41"/>
       <c r="B127" s="20" t="s">
         <v>53</v>
@@ -7026,7 +7047,7 @@
         <v>44215</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="41"/>
       <c r="B128" s="20" t="s">
         <v>55</v>
@@ -7048,7 +7069,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="41"/>
       <c r="B129" s="20" t="s">
         <v>71</v>
@@ -7070,7 +7091,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="41"/>
       <c r="B130" s="20" t="s">
         <v>57</v>
@@ -7092,7 +7113,7 @@
         <v>44229</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="41">
         <v>44378</v>
       </c>
@@ -7116,7 +7137,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="41"/>
       <c r="B132" s="20" t="s">
         <v>55</v>
@@ -7138,7 +7159,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="41"/>
       <c r="B133" s="20" t="s">
         <v>55</v>
@@ -7160,7 +7181,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="41">
         <v>44440</v>
       </c>
@@ -7182,7 +7203,7 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="41">
         <v>44470</v>
       </c>
@@ -7206,7 +7227,7 @@
         <v>44489</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="41"/>
       <c r="B136" s="20" t="s">
         <v>136</v>
@@ -7228,7 +7249,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="41"/>
       <c r="B137" s="20" t="s">
         <v>121</v>
@@ -7248,7 +7269,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="47" t="s">
         <v>52</v>
       </c>
@@ -7266,7 +7287,7 @@
       <c r="J138" s="11"/>
       <c r="K138" s="20"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="41">
         <v>44562</v>
       </c>
@@ -7290,7 +7311,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="41"/>
       <c r="B140" s="20" t="s">
         <v>57</v>
@@ -7312,7 +7333,7 @@
         <v>44589</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="41"/>
       <c r="B141" s="20" t="s">
         <v>55</v>
@@ -7334,7 +7355,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="41">
         <v>44593</v>
       </c>
@@ -7358,7 +7379,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="41"/>
       <c r="B143" s="20" t="s">
         <v>55</v>
@@ -7380,7 +7401,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="41"/>
       <c r="B144" s="20" t="s">
         <v>71</v>
@@ -7402,7 +7423,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="41"/>
       <c r="B145" s="20" t="s">
         <v>55</v>
@@ -7424,7 +7445,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="41">
         <v>44652</v>
       </c>
@@ -7448,7 +7469,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="41"/>
       <c r="B147" s="20" t="s">
         <v>57</v>
@@ -7470,7 +7491,7 @@
         <v>44680</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="41">
         <v>44682</v>
       </c>
@@ -7494,7 +7515,7 @@
         <v>44704</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="41">
         <v>44713</v>
       </c>
@@ -7516,7 +7537,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="41"/>
       <c r="B150" s="20" t="s">
         <v>55</v>
@@ -7538,7 +7559,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="41"/>
       <c r="B151" s="20" t="s">
         <v>57</v>
@@ -7560,7 +7581,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="41"/>
       <c r="B152" s="20" t="s">
         <v>57</v>
@@ -7582,7 +7603,7 @@
         <v>44764</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="41"/>
       <c r="B153" s="20" t="s">
         <v>55</v>
@@ -7604,7 +7625,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="41"/>
       <c r="B154" s="20" t="s">
         <v>55</v>
@@ -7626,7 +7647,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="41">
         <v>44805</v>
       </c>
@@ -7650,7 +7671,7 @@
         <v>44811</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="41"/>
       <c r="B156" s="20" t="s">
         <v>57</v>
@@ -7672,7 +7693,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="41">
         <v>44835</v>
       </c>
@@ -7696,7 +7717,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="41"/>
       <c r="B158" s="20" t="s">
         <v>57</v>
@@ -7718,7 +7739,7 @@
         <v>44841</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="41"/>
       <c r="B159" s="20" t="s">
         <v>53</v>
@@ -7738,7 +7759,7 @@
         <v>44845</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="41"/>
       <c r="B160" s="20" t="s">
         <v>57</v>
@@ -7760,7 +7781,7 @@
         <v>44854</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="41"/>
       <c r="B161" s="20" t="s">
         <v>55</v>
@@ -7782,7 +7803,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="41">
         <v>44866</v>
       </c>
@@ -7804,7 +7825,7 @@
         <v>44893</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="41"/>
       <c r="B163" s="20" t="s">
         <v>57</v>
@@ -7826,7 +7847,7 @@
         <v>44876</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="41"/>
       <c r="B164" s="20" t="s">
         <v>57</v>
@@ -7848,7 +7869,7 @@
         <v>44887</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="41">
         <v>44896</v>
       </c>
@@ -7872,7 +7893,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="47" t="s">
         <v>145</v>
       </c>
@@ -7890,7 +7911,7 @@
       <c r="J166" s="11"/>
       <c r="K166" s="20"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="41">
         <v>44986</v>
       </c>
@@ -7914,7 +7935,7 @@
         <v>44995</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="41">
         <v>45017</v>
       </c>
@@ -7938,7 +7959,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="41">
         <v>45047</v>
       </c>
@@ -7956,7 +7977,7 @@
       <c r="J169" s="11"/>
       <c r="K169" s="20"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="41">
         <v>45078</v>
       </c>
@@ -7980,7 +8001,7 @@
         <v>45082</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="41">
         <v>45139</v>
       </c>
@@ -8004,7 +8025,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="41"/>
       <c r="B172" s="20" t="s">
         <v>57</v>
@@ -8026,7 +8047,7 @@
         <v>45167</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="41">
         <v>45170</v>
       </c>
@@ -8050,7 +8071,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="41">
         <v>45200</v>
       </c>
@@ -8074,7 +8095,7 @@
         <v>45223</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="41"/>
       <c r="B175" s="20" t="s">
         <v>57</v>
@@ -8096,7 +8117,7 @@
         <v>45230</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="41"/>
       <c r="B176" s="20"/>
       <c r="C176" s="13"/>
@@ -8112,7 +8133,7 @@
       <c r="J176" s="11"/>
       <c r="K176" s="20"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="41"/>
       <c r="B177" s="20"/>
       <c r="C177" s="13"/>
@@ -8128,7 +8149,7 @@
       <c r="J177" s="11"/>
       <c r="K177" s="20"/>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="41"/>
       <c r="B178" s="20"/>
       <c r="C178" s="13"/>
@@ -8144,7 +8165,7 @@
       <c r="J178" s="11"/>
       <c r="K178" s="20"/>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="41"/>
       <c r="B179" s="20"/>
       <c r="C179" s="13"/>
@@ -8160,7 +8181,7 @@
       <c r="J179" s="11"/>
       <c r="K179" s="20"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="41"/>
       <c r="B180" s="20"/>
       <c r="C180" s="13"/>
@@ -8176,7 +8197,7 @@
       <c r="J180" s="11"/>
       <c r="K180" s="20"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="41"/>
       <c r="B181" s="20"/>
       <c r="C181" s="13"/>
@@ -8192,7 +8213,7 @@
       <c r="J181" s="11"/>
       <c r="K181" s="20"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="41"/>
       <c r="B182" s="20"/>
       <c r="C182" s="13"/>
@@ -8208,7 +8229,7 @@
       <c r="J182" s="11"/>
       <c r="K182" s="20"/>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="41"/>
       <c r="B183" s="20"/>
       <c r="C183" s="13"/>
@@ -8224,7 +8245,7 @@
       <c r="J183" s="11"/>
       <c r="K183" s="20"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="41"/>
       <c r="B184" s="20"/>
       <c r="C184" s="13"/>
@@ -8240,7 +8261,7 @@
       <c r="J184" s="11"/>
       <c r="K184" s="20"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="41"/>
       <c r="B185" s="20"/>
       <c r="C185" s="13"/>
@@ -8256,7 +8277,7 @@
       <c r="J185" s="11"/>
       <c r="K185" s="20"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="41"/>
       <c r="B186" s="20"/>
       <c r="C186" s="13"/>
@@ -8272,7 +8293,7 @@
       <c r="J186" s="11"/>
       <c r="K186" s="20"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="41"/>
       <c r="B187" s="20"/>
       <c r="C187" s="13"/>
@@ -8288,7 +8309,7 @@
       <c r="J187" s="11"/>
       <c r="K187" s="20"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="41"/>
       <c r="B188" s="20"/>
       <c r="C188" s="13"/>
@@ -8304,7 +8325,7 @@
       <c r="J188" s="11"/>
       <c r="K188" s="20"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="41"/>
       <c r="B189" s="20"/>
       <c r="C189" s="13"/>
@@ -8320,7 +8341,7 @@
       <c r="J189" s="11"/>
       <c r="K189" s="20"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="41"/>
       <c r="B190" s="20"/>
       <c r="C190" s="13"/>
@@ -8336,7 +8357,7 @@
       <c r="J190" s="11"/>
       <c r="K190" s="20"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="41"/>
       <c r="B191" s="20"/>
       <c r="C191" s="13"/>
@@ -8352,7 +8373,7 @@
       <c r="J191" s="11"/>
       <c r="K191" s="20"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="41"/>
       <c r="B192" s="20"/>
       <c r="C192" s="13"/>
@@ -8368,7 +8389,7 @@
       <c r="J192" s="11"/>
       <c r="K192" s="20"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="41"/>
       <c r="B193" s="20"/>
       <c r="C193" s="13"/>
@@ -8384,7 +8405,7 @@
       <c r="J193" s="11"/>
       <c r="K193" s="20"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="41"/>
       <c r="B194" s="20"/>
       <c r="C194" s="13"/>
@@ -8400,7 +8421,7 @@
       <c r="J194" s="11"/>
       <c r="K194" s="20"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="41"/>
       <c r="B195" s="20"/>
       <c r="C195" s="13"/>
@@ -8416,7 +8437,7 @@
       <c r="J195" s="11"/>
       <c r="K195" s="20"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="41"/>
       <c r="B196" s="20"/>
       <c r="C196" s="13"/>
@@ -8432,7 +8453,7 @@
       <c r="J196" s="11"/>
       <c r="K196" s="20"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="41"/>
       <c r="B197" s="20"/>
       <c r="C197" s="13"/>
@@ -8448,7 +8469,7 @@
       <c r="J197" s="11"/>
       <c r="K197" s="20"/>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="41"/>
       <c r="B198" s="20"/>
       <c r="C198" s="13"/>
@@ -8464,7 +8485,7 @@
       <c r="J198" s="11"/>
       <c r="K198" s="20"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="41"/>
       <c r="B199" s="20"/>
       <c r="C199" s="13"/>
@@ -8480,7 +8501,7 @@
       <c r="J199" s="11"/>
       <c r="K199" s="20"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="41"/>
       <c r="B200" s="20"/>
       <c r="C200" s="13"/>
@@ -8496,7 +8517,7 @@
       <c r="J200" s="11"/>
       <c r="K200" s="20"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="41"/>
       <c r="B201" s="20"/>
       <c r="C201" s="13"/>
@@ -8512,7 +8533,7 @@
       <c r="J201" s="11"/>
       <c r="K201" s="20"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="41"/>
       <c r="B202" s="20"/>
       <c r="C202" s="13"/>
@@ -8528,7 +8549,7 @@
       <c r="J202" s="11"/>
       <c r="K202" s="20"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="41"/>
       <c r="B203" s="20"/>
       <c r="C203" s="13"/>
@@ -8544,7 +8565,7 @@
       <c r="J203" s="11"/>
       <c r="K203" s="20"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="42"/>
       <c r="B204" s="15"/>
       <c r="C204" s="43"/>
@@ -8575,10 +8596,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8601,28 +8622,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="38" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="38" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -8635,7 +8656,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -8664,7 +8685,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>53.343000000000004</v>
       </c>
@@ -8696,7 +8717,7 @@
         <v>0.20799999999999974</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E4" s="1">
         <f>IF(E3=0,0,IF(ISBLANK(E3),"",VLOOKUP(E3,E7:F14,2)))</f>
         <v>0</v>
@@ -8711,10 +8732,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="39" t="s">
         <v>28</v>
       </c>
@@ -8734,7 +8755,7 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="38">
         <v>1</v>
       </c>
@@ -8760,7 +8781,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="38">
         <v>2</v>
       </c>
@@ -8786,7 +8807,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="38">
         <v>3</v>
       </c>
@@ -8812,7 +8833,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="38">
         <v>4</v>
       </c>
@@ -8838,7 +8859,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="38">
         <v>5</v>
       </c>
@@ -8864,7 +8885,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="38">
         <v>6</v>
       </c>
@@ -8890,7 +8911,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="38">
         <v>7</v>
       </c>
@@ -8916,7 +8937,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="38">
         <v>8</v>
       </c>
@@ -8942,7 +8963,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="38">
         <v>9</v>
       </c>
@@ -8962,7 +8983,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="38">
         <v>10</v>
       </c>
@@ -8982,7 +9003,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="38">
         <v>11</v>
       </c>
@@ -9002,7 +9023,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="38">
         <v>12</v>
       </c>
@@ -9023,7 +9044,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="38">
         <v>13</v>
       </c>
@@ -9044,7 +9065,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="38">
         <v>14</v>
       </c>
@@ -9065,7 +9086,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="38">
         <v>15</v>
       </c>
@@ -9086,7 +9107,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="38">
         <v>16</v>
       </c>
@@ -9107,7 +9128,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="38">
         <v>17</v>
       </c>
@@ -9128,7 +9149,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="38">
         <v>18</v>
       </c>
@@ -9149,7 +9170,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="38">
         <v>19</v>
       </c>
@@ -9170,7 +9191,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="38">
         <v>20</v>
       </c>
@@ -9191,7 +9212,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="38">
         <v>21</v>
       </c>
@@ -9212,7 +9233,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="38">
         <v>22</v>
       </c>
@@ -9233,7 +9254,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="38">
         <v>23</v>
       </c>
@@ -9254,7 +9275,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="38">
         <v>24</v>
       </c>
@@ -9275,7 +9296,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="38">
         <v>25</v>
       </c>
@@ -9296,7 +9317,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="38">
         <v>26</v>
       </c>
@@ -9317,7 +9338,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="38">
         <v>27</v>
       </c>
@@ -9338,7 +9359,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="38">
         <v>28</v>
       </c>
@@ -9359,7 +9380,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="38">
         <v>29</v>
       </c>
@@ -9380,7 +9401,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="38">
         <v>30</v>
       </c>
@@ -9401,7 +9422,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="38">
         <v>31</v>
       </c>
@@ -9422,7 +9443,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="38">
         <v>32</v>
       </c>
@@ -9431,7 +9452,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="38">
         <v>33</v>
       </c>
@@ -9440,7 +9461,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="38">
         <v>34</v>
       </c>
@@ -9449,7 +9470,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="38">
         <v>35</v>
       </c>
@@ -9458,7 +9479,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="38">
         <v>36</v>
       </c>
@@ -9467,7 +9488,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="38">
         <v>37</v>
       </c>
@@ -9476,7 +9497,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="38">
         <v>38</v>
       </c>
@@ -9485,7 +9506,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="38">
         <v>39</v>
       </c>
@@ -9494,7 +9515,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="38">
         <v>40</v>
       </c>
@@ -9503,7 +9524,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="38">
         <v>41</v>
       </c>
@@ -9512,7 +9533,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="38">
         <v>42</v>
       </c>
@@ -9521,7 +9542,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="38">
         <v>43</v>
       </c>
@@ -9530,7 +9551,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="38">
         <v>44</v>
       </c>
@@ -9539,7 +9560,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="38">
         <v>45</v>
       </c>
@@ -9548,7 +9569,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="38">
         <v>46</v>
       </c>
@@ -9557,7 +9578,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="38">
         <v>47</v>
       </c>
@@ -9566,7 +9587,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="38">
         <v>48</v>
       </c>
@@ -9575,7 +9596,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="38">
         <v>49</v>
       </c>
@@ -9584,7 +9605,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="38">
         <v>50</v>
       </c>
@@ -9593,7 +9614,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="38">
         <v>51</v>
       </c>
@@ -9602,7 +9623,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="38">
         <v>52</v>
       </c>
@@ -9611,7 +9632,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="38">
         <v>53</v>
       </c>
@@ -9620,7 +9641,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="38">
         <v>54</v>
       </c>
@@ -9629,7 +9650,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="38">
         <v>55</v>
       </c>
@@ -9638,7 +9659,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="38">
         <v>56</v>
       </c>
@@ -9647,7 +9668,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="38">
         <v>57</v>
       </c>
@@ -9656,7 +9677,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="38">
         <v>58</v>
       </c>
@@ -9665,7 +9686,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="38">
         <v>59</v>
       </c>
@@ -9674,7 +9695,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="38">
         <v>60</v>
       </c>
@@ -9683,7 +9704,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>